<commit_message>
resolved the easy requirements
</commit_message>
<xml_diff>
--- a/Requirements/m2w initial feedback.xlsx
+++ b/Requirements/m2w initial feedback.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
   <si>
     <t>Purchase Order screen:</t>
   </si>
@@ -35,13 +35,16 @@
     <t>medium</t>
   </si>
   <si>
-    <t>database change</t>
+    <t>Screen/field validation change</t>
   </si>
   <si>
     <t>done</t>
   </si>
   <si>
     <t>Allow for entry of weight for total PO to 2 decimal places (ei: 100.25 T)(This is a required field)</t>
+  </si>
+  <si>
+    <t>database change</t>
   </si>
   <si>
     <t>Weight of tonnage calculated into pounds by *2206.7. (ei 100.25 * 2206.7 = 221151.5) however this will be rounded to the nearest 10 lbs, so the example would be 221,152 lbs.</t>
@@ -354,7 +357,7 @@
   <dimension ref="1:35"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2442,9 +2445,11 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
-      <c r="D3" s="0"/>
+      <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="E3" s="0"/>
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
@@ -3468,7 +3473,7 @@
     </row>
     <row r="4" s="3" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -3476,13 +3481,13 @@
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="0"/>
       <c r="E5" s="0"/>
@@ -4508,13 +4513,13 @@
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
@@ -5542,13 +5547,13 @@
     </row>
     <row r="7" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" s="0"/>
       <c r="E7" s="0"/>
@@ -6574,13 +6579,13 @@
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="0"/>
       <c r="E8" s="0"/>
@@ -7606,11 +7611,11 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0"/>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
@@ -8639,7 +8644,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="3"/>
@@ -9667,15 +9672,17 @@
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
-      <c r="D12" s="0"/>
+      <c r="D12" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
@@ -10699,13 +10706,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" s="0"/>
       <c r="E13" s="0"/>
@@ -11731,10 +11738,10 @@
     </row>
     <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>7</v>
@@ -11742,13 +11749,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D15" s="0"/>
       <c r="E15" s="0"/>
@@ -12774,13 +12781,13 @@
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D16" s="0"/>
       <c r="E16" s="0"/>
@@ -13806,13 +13813,13 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D17" s="0"/>
       <c r="E17" s="0"/>
@@ -14838,13 +14845,13 @@
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D18" s="0"/>
       <c r="E18" s="0"/>
@@ -15870,11 +15877,11 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B19" s="0"/>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D19" s="0"/>
       <c r="E19" s="0"/>
@@ -16900,13 +16907,13 @@
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D20" s="0"/>
       <c r="E20" s="0"/>
@@ -17932,13 +17939,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>7</v>
@@ -18969,7 +18976,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23" s="0"/>
       <c r="C23" s="3"/>
@@ -19997,10 +20004,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C24" s="0"/>
       <c r="D24" s="0" t="s">
@@ -21029,10 +21036,10 @@
     </row>
     <row r="25" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>7</v>
@@ -21040,7 +21047,7 @@
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>5</v>
@@ -22070,10 +22077,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="0"/>
       <c r="D27" s="0" t="s">
@@ -23102,13 +23109,13 @@
     </row>
     <row r="28" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D28" s="0"/>
       <c r="E28" s="0"/>
@@ -24134,13 +24141,13 @@
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D29" s="0"/>
       <c r="E29" s="0"/>
@@ -25166,7 +25173,7 @@
     </row>
     <row r="30" s="3" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>5</v>
@@ -25174,13 +25181,13 @@
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D31" s="0"/>
       <c r="E31" s="0"/>
@@ -26206,16 +26213,16 @@
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E32" s="0"/>
       <c r="F32" s="0"/>
@@ -27240,13 +27247,13 @@
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D33" s="0"/>
       <c r="E33" s="0"/>
@@ -28272,7 +28279,7 @@
     </row>
     <row r="34" s="3" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>5</v>
@@ -28280,13 +28287,13 @@
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed medium rail car
</commit_message>
<xml_diff>
--- a/Requirements/m2w initial feedback.xlsx
+++ b/Requirements/m2w initial feedback.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
   <si>
     <t>Purchase Order screen:</t>
   </si>
@@ -80,6 +80,9 @@
     <t>No data is entered if user does nor complete the screen</t>
   </si>
   <si>
+    <t>done?</t>
+  </si>
+  <si>
     <t>The layout below: Check screen</t>
   </si>
   <si>
@@ -110,7 +113,7 @@
     <t>Vendor PO number should be Halliburton TO# (10-15 digits)</t>
   </si>
   <si>
-    <t>need to work on Po #</t>
+    <t>need to work on Po #, integers max is 10 digits, database</t>
   </si>
   <si>
     <t>Purchase order should be a drop down from those PO's that have a remaining balance &gt;100lbs.</t>
@@ -357,7 +360,7 @@
   <dimension ref="1:35"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3478,6 +3481,9 @@
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -6587,7 +6593,9 @@
       <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="0"/>
+      <c r="D8" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
@@ -7611,11 +7619,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
-      <c r="B9" s="0"/>
+      <c r="B9" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
@@ -8644,7 +8654,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="3"/>
@@ -9672,7 +9682,7 @@
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>5</v>
@@ -10706,7 +10716,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>5</v>
@@ -10714,7 +10724,9 @@
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="0"/>
+      <c r="D13" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
@@ -11738,10 +11750,10 @@
     </row>
     <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>7</v>
@@ -11749,15 +11761,17 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
-      <c r="D15" s="0"/>
+      <c r="D15" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="E15" s="0"/>
       <c r="F15" s="0"/>
       <c r="G15" s="0"/>
@@ -12781,13 +12795,13 @@
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D16" s="0"/>
       <c r="E16" s="0"/>
@@ -13813,7 +13827,7 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -15877,11 +15891,11 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19" s="0"/>
       <c r="C19" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D19" s="0"/>
       <c r="E19" s="0"/>
@@ -16907,13 +16921,13 @@
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D20" s="0"/>
       <c r="E20" s="0"/>
@@ -17939,13 +17953,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>7</v>
@@ -18976,7 +18990,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B23" s="0"/>
       <c r="C23" s="3"/>
@@ -20004,10 +20018,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C24" s="0"/>
       <c r="D24" s="0" t="s">
@@ -21036,10 +21050,10 @@
     </row>
     <row r="25" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>7</v>
@@ -21047,7 +21061,7 @@
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>5</v>
@@ -22077,10 +22091,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C27" s="0"/>
       <c r="D27" s="0" t="s">
@@ -23109,13 +23123,13 @@
     </row>
     <row r="28" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D28" s="0"/>
       <c r="E28" s="0"/>
@@ -24141,13 +24155,13 @@
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D29" s="0"/>
       <c r="E29" s="0"/>
@@ -25173,7 +25187,7 @@
     </row>
     <row r="30" s="3" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>5</v>
@@ -25181,13 +25195,13 @@
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D31" s="0"/>
       <c r="E31" s="0"/>
@@ -26213,16 +26227,16 @@
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E32" s="0"/>
       <c r="F32" s="0"/>
@@ -27247,13 +27261,13 @@
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D33" s="0"/>
       <c r="E33" s="0"/>
@@ -28279,7 +28293,7 @@
     </row>
     <row r="34" s="3" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>5</v>
@@ -28287,13 +28301,13 @@
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added file uploads to amazaon for trailer
</commit_message>
<xml_diff>
--- a/Requirements/m2w initial feedback.xlsx
+++ b/Requirements/m2w initial feedback.xlsx
@@ -5,17 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="72">
   <si>
     <t>Purchase Order screen:</t>
   </si>
@@ -41,6 +41,9 @@
     <t>done</t>
   </si>
   <si>
+    <t>Approved</t>
+  </si>
+  <si>
     <t>Allow for entry of weight for total PO to 2 decimal places (ei: 100.25 T)(This is a required field)</t>
   </si>
   <si>
@@ -48,6 +51,9 @@
   </si>
   <si>
     <t>Weight of tonnage calculated into pounds by *2206.7. (ei 100.25 * 2206.7 = 221151.5) however this will be rounded to the nearest 10 lbs, so the example would be 221,152 lbs.</t>
+  </si>
+  <si>
+    <t>This doesn't round correctly, for 100.25T should read 221160lbs, needs to round to the nearest 10lbs.</t>
   </si>
   <si>
     <t>Drop down menu for “vendor” – and a table that contains them so users can add them.</t>
@@ -74,6 +80,9 @@
     <t>I'll have to check the Access DB how this is done</t>
   </si>
   <si>
+    <t>Calculation is PO# Tonnage - Trailered Tons = Remaining weight</t>
+  </si>
+  <si>
     <t>Not allow for the user to click the back button, I need it to crash/not load a screen.</t>
   </si>
   <si>
@@ -81,6 +90,9 @@
   </si>
   <si>
     <t>done?</t>
+  </si>
+  <si>
+    <t>The back button in the explorer window should not load the page again.</t>
   </si>
   <si>
     <t>The layout below: Check screen</t>
@@ -95,7 +107,13 @@
     <t>Weight on arrival should show “Weight on arrival in Tons”, “Weight at origin in Tons” Needs to allow for two decimal’s .</t>
   </si>
   <si>
+    <t>Errored out / not approved.</t>
+  </si>
+  <si>
     <t>Sand Grade should be a drop down</t>
+  </si>
+  <si>
+    <t>Approved.</t>
   </si>
   <si>
     <t>BOL Number 8-10 digits</t>
@@ -119,6 +137,9 @@
     <t>Purchase order should be a drop down from those PO's that have a remaining balance &gt;100lbs.</t>
   </si>
   <si>
+    <t>Any remaining weight on the PO &gt;100lbs (.5T) display the PO in the drop down.'</t>
+  </si>
+  <si>
     <t>DB</t>
   </si>
   <si>
@@ -128,7 +149,10 @@
     <t>Maybe we can remove some fields, what is the min requirement to display?</t>
   </si>
   <si>
-    <t>Done </t>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Approved, but more lateral look vs Vertical.</t>
   </si>
   <si>
     <t>Allow for a scanned document to be uploaded.</t>
@@ -137,16 +161,22 @@
     <t>Need to research on uploads and keeping them on the server for reference</t>
   </si>
   <si>
-    <t>Rails car Nb # </t>
+    <t>Rails car Nb #</t>
   </si>
   <si>
     <t>Mandatory, added by CL</t>
+  </si>
+  <si>
+    <t>Created by/edited by should be automatically entered, system requires entry.</t>
   </si>
   <si>
     <t>New Trailer:</t>
   </si>
   <si>
     <t>Trailer Number (required field)</t>
+  </si>
+  <si>
+    <t>approved</t>
   </si>
   <si>
     <t>Driver name (Required field)</t>
@@ -158,13 +188,13 @@
     <t>BOL number should be entered by the user (required)</t>
   </si>
   <si>
-    <t>Time in and Time out should be buttons, Time in first when clicked time stamp the record, and time out is greyed out. Once time in is clicked time out is allowed to be clicked. (This is HH:MM:SS  DD:MM:YY) format. </t>
+    <t>Time in and Time out should be buttons, Time in first when clicked time stamp the record, and time out is greyed out. Once time in is clicked time out is allowed to be clicked. (This is HH:MM:SS  DD:MM:YY) format.</t>
   </si>
   <si>
     <t>need work on how to work conditionals on screen</t>
   </si>
   <si>
-    <t>Rail car = from rail car screen (with only those rail cars who are not clicked as ‘empty car’). </t>
+    <t>Rail car = from rail car screen (with only those rail cars who are not clicked as ‘empty car’).</t>
   </si>
   <si>
     <t>to research</t>
@@ -188,7 +218,10 @@
     <t>made weight_lbs mandatory</t>
   </si>
   <si>
-    <t>Purchase order should be a drop down based on the entries from the Create new PO screen. </t>
+    <t>Weight in tons should be calculated based on User entry, like with the PO Screen.</t>
+  </si>
+  <si>
+    <t>Purchase order should be a drop down based on the entries from the Create new PO screen.</t>
   </si>
   <si>
     <t>Then once this entry takes place, to subtract the tonnage from the Purchase order, and display the ‘remaining balance’ in the purchase order screen.</t>
@@ -212,6 +245,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -233,18 +267,21 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -252,14 +289,21 @@
       <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -296,7 +340,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -314,31 +358,67 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -358,22 +438,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:35"/>
+  <dimension ref="1:36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.484693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="16.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="46.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="46.4438775510204"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="3" width="18.8877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.3367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="3" width="11.5561224489796"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -386,7 +467,7 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0"/>
+      <c r="E1" s="7"/>
       <c r="F1" s="0"/>
       <c r="G1" s="0"/>
       <c r="H1" s="0"/>
@@ -1407,20 +1488,22 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="0"/>
+      <c r="E2" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
@@ -2441,20 +2524,22 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="0"/>
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
@@ -3475,29 +3560,35 @@
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="3" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
+    <row r="4" customFormat="false" ht="52.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="E4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="0"/>
-      <c r="E5" s="0"/>
+      <c r="B5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0"/>
       <c r="H5" s="0"/>
@@ -4518,20 +4609,22 @@
       <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
+    <row r="6" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
+      <c r="C6" s="8" t="s">
+        <v>17</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="0"/>
+      <c r="E6" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="F6" s="0"/>
       <c r="G6" s="0"/>
       <c r="H6" s="0"/>
@@ -5552,18 +5645,20 @@
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="s">
+    <row r="7" customFormat="false" ht="105.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
+      <c r="B7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F7" s="0"/>
       <c r="G7" s="0"/>
       <c r="H7" s="0"/>
@@ -6584,20 +6679,22 @@
       <c r="AMI7" s="0"/>
       <c r="AMJ7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
+    <row r="8" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>22</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
+      <c r="B8" s="9" t="s">
+        <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
+      <c r="C8" s="8" t="s">
+        <v>23</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>21</v>
+      <c r="D8" s="10" t="s">
+        <v>24</v>
       </c>
-      <c r="E8" s="0"/>
+      <c r="E8" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
       <c r="H8" s="0"/>
@@ -7618,18 +7715,18 @@
       <c r="AMI8" s="0"/>
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
+    <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>26</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
+      <c r="C9" s="8" t="s">
+        <v>27</v>
       </c>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
       <c r="H9" s="0"/>
@@ -8650,17 +8747,21 @@
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="2"/>
+    <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="8"/>
     </row>
-    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
-      <c r="B11" s="0"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="0"/>
-      <c r="E11" s="0"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
       <c r="H11" s="0"/>
@@ -9681,20 +9782,22 @@
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
+    <row r="12" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>29</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>9</v>
+      <c r="C12" s="8" t="s">
+        <v>10</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="0"/>
+      <c r="E12" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
       <c r="H12" s="0"/>
@@ -10715,20 +10818,22 @@
       <c r="AMI12" s="0"/>
       <c r="AMJ12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
+    <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>31</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>15</v>
+      <c r="C13" s="8" t="s">
+        <v>17</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="0"/>
+      <c r="E13" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
@@ -11749,31 +11854,37 @@
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
+    <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>33</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>28</v>
+      <c r="B14" s="9" t="s">
+        <v>34</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="E14" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>29</v>
+    <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>35</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>30</v>
+      <c r="C15" s="8" t="s">
+        <v>36</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="0"/>
+      <c r="E15" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="F15" s="0"/>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
@@ -12794,20 +12905,22 @@
       <c r="AMI15" s="0"/>
       <c r="AMJ15" s="0"/>
     </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>31</v>
+    <row r="16" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>37</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>17</v>
+      <c r="B16" s="9" t="s">
+        <v>19</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="0"/>
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
@@ -13828,18 +13941,20 @@
       <c r="AMI16" s="0"/>
       <c r="AMJ16" s="0"/>
     </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>33</v>
+    <row r="17" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>39</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>15</v>
+      <c r="D17" s="10"/>
+      <c r="E17" s="7" t="s">
+        <v>40</v>
       </c>
-      <c r="D17" s="0"/>
-      <c r="E17" s="0"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
@@ -14860,18 +14975,18 @@
       <c r="AMI17" s="0"/>
       <c r="AMJ17" s="0"/>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>34</v>
+    <row r="18" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>41</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>12</v>
+      <c r="B18" s="9" t="s">
+        <v>14</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>20</v>
+      <c r="C18" s="8" t="s">
+        <v>23</v>
       </c>
-      <c r="D18" s="0"/>
-      <c r="E18" s="0"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
@@ -15892,18 +16007,20 @@
       <c r="AMI18" s="0"/>
       <c r="AMJ18" s="0"/>
     </row>
-    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>35</v>
+    <row r="19" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>42</v>
       </c>
-      <c r="B19" s="0"/>
-      <c r="C19" s="1" t="s">
-        <v>36</v>
+      <c r="B19" s="10"/>
+      <c r="C19" s="8" t="s">
+        <v>43</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>37</v>
+      <c r="D19" s="10" t="s">
+        <v>44</v>
       </c>
-      <c r="E19" s="0"/>
+      <c r="E19" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="F19" s="0"/>
       <c r="G19" s="0"/>
       <c r="H19" s="0"/>
@@ -16924,18 +17041,20 @@
       <c r="AMI19" s="0"/>
       <c r="AMJ19" s="0"/>
     </row>
-    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>38</v>
+    <row r="20" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>46</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>17</v>
+      <c r="B20" s="9" t="s">
+        <v>19</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>39</v>
+      <c r="C20" s="8" t="s">
+        <v>47</v>
       </c>
-      <c r="D20" s="0"/>
-      <c r="E20" s="0"/>
+      <c r="D20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="7"/>
       <c r="F20" s="0"/>
       <c r="G20" s="0"/>
       <c r="H20" s="0"/>
@@ -17956,20 +18075,22 @@
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>40</v>
+    <row r="21" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="11" t="s">
+        <v>48</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>28</v>
+      <c r="B21" s="12" t="s">
+        <v>34</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>41</v>
+      <c r="C21" s="13" t="s">
+        <v>49</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="0"/>
+      <c r="E21" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="F21" s="0"/>
       <c r="G21" s="0"/>
       <c r="H21" s="0"/>
@@ -18990,17 +19111,21 @@
       <c r="AMI21" s="0"/>
       <c r="AMJ21" s="0"/>
     </row>
-    <row r="22" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="2"/>
+    <row r="22" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="19"/>
     </row>
-    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="0"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="0"/>
-      <c r="E23" s="0"/>
+    <row r="23" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="8"/>
       <c r="F23" s="0"/>
       <c r="G23" s="0"/>
       <c r="H23" s="0"/>
@@ -20021,18 +20146,14 @@
       <c r="AMI23" s="0"/>
       <c r="AMJ23" s="0"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>43</v>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>51</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="0"/>
-      <c r="D24" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="0"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="0"/>
       <c r="G24" s="0"/>
       <c r="H24" s="0"/>
@@ -21053,27 +21174,35 @@
       <c r="AMI24" s="0"/>
       <c r="AMJ24" s="0"/>
     </row>
-    <row r="25" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>44</v>
+    <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
+        <v>52</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>28</v>
+      <c r="B25" s="9" t="s">
+        <v>34</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="C25" s="10"/>
+      <c r="D25" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="E25" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>45</v>
+    <row r="26" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>54</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>5</v>
+      <c r="B26" s="9" t="s">
+        <v>34</v>
       </c>
-      <c r="C26" s="0"/>
-      <c r="D26" s="0"/>
-      <c r="E26" s="0"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="F26" s="0"/>
       <c r="G26" s="0"/>
       <c r="H26" s="0"/>
@@ -22094,18 +22223,16 @@
       <c r="AMI26" s="0"/>
       <c r="AMJ26" s="0"/>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>46</v>
+    <row r="27" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
+        <v>55</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>28</v>
+      <c r="B27" s="9" t="s">
+        <v>5</v>
       </c>
-      <c r="C27" s="0"/>
-      <c r="D27" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="0"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="7"/>
       <c r="F27" s="0"/>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
@@ -23126,18 +23253,20 @@
       <c r="AMI27" s="0"/>
       <c r="AMJ27" s="0"/>
     </row>
-    <row r="28" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>47</v>
+    <row r="28" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
+        <v>56</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>17</v>
+      <c r="B28" s="9" t="s">
+        <v>34</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>48</v>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10" t="s">
+        <v>7</v>
       </c>
-      <c r="D28" s="0"/>
-      <c r="E28" s="0"/>
+      <c r="E28" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="F28" s="0"/>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
@@ -24158,18 +24287,18 @@
       <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
     </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>49</v>
+    <row r="29" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
+        <v>57</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>17</v>
+      <c r="B29" s="9" t="s">
+        <v>19</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>50</v>
+      <c r="C29" s="8" t="s">
+        <v>58</v>
       </c>
-      <c r="D29" s="0"/>
-      <c r="E29" s="0"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="7"/>
       <c r="F29" s="0"/>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
@@ -25190,26 +25319,29 @@
       <c r="AMI29" s="0"/>
       <c r="AMJ29" s="0"/>
     </row>
-    <row r="30" s="3" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>51</v>
+    <row r="30" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>59</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" customFormat="false" ht="52.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="0"/>
-      <c r="E31" s="0"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="8"/>
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
       <c r="H31" s="0"/>
@@ -26230,20 +26362,18 @@
       <c r="AMI31" s="0"/>
       <c r="AMJ31" s="0"/>
     </row>
-    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>54</v>
+    <row r="32" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="8" t="s">
+        <v>62</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>55</v>
+      <c r="C32" s="8" t="s">
+        <v>63</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E32" s="0"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="7"/>
       <c r="F32" s="0"/>
       <c r="G32" s="0"/>
       <c r="H32" s="0"/>
@@ -27264,18 +27394,22 @@
       <c r="AMI32" s="0"/>
       <c r="AMJ32" s="0"/>
     </row>
-    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>57</v>
+    <row r="33" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="s">
+        <v>64</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>55</v>
+      <c r="C33" s="8" t="s">
+        <v>65</v>
       </c>
-      <c r="D33" s="0"/>
-      <c r="E33" s="0"/>
+      <c r="D33" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>67</v>
+      </c>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
       <c r="H33" s="0"/>
@@ -28296,29 +28430,47 @@
       <c r="AMI33" s="0"/>
       <c r="AMJ33" s="0"/>
     </row>
-    <row r="34" s="3" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>58</v>
+    <row r="34" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
+        <v>68</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="9" t="s">
         <v>5</v>
       </c>
+      <c r="C34" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="10"/>
+      <c r="E34" s="7"/>
     </row>
-    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>59</v>
+    <row r="35" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="8" t="s">
+        <v>69</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>60</v>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="8" t="s">
+        <v>70</v>
       </c>
+      <c r="B36" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="10"/>
+      <c r="E36" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
po now displays on show screen
</commit_message>
<xml_diff>
--- a/Requirements/m2w initial feedback.xlsx
+++ b/Requirements/m2w initial feedback.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="72">
   <si>
     <t>Purchase Order screen:</t>
   </si>
@@ -440,8 +440,8 @@
   </sheetPr>
   <dimension ref="1:36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -34558,7 +34558,9 @@
       <c r="C34" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="10"/>
+      <c r="D34" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fixed PO on rail car, added states drop down, changed datatype for weight at origin in rail car, removed calculated fields from edit screens
</commit_message>
<xml_diff>
--- a/Requirements/m2w initial feedback.xlsx
+++ b/Requirements/m2w initial feedback.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
   <si>
     <t>Purchase Order screen:</t>
   </si>
@@ -51,6 +51,30 @@
   </si>
   <si>
     <t>Weight of tonnage calculated into pounds by *2206.7. (ei 100.25 * 2206.7 = 221151.5) however this will be rounded to the nearest 10 lbs, so the example would be 221,152 lbs.</t>
+  </si>
+  <si>
+    <r>
+      <t>did with rounding to nearest 10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t> decimal – done</t>
+    </r>
   </si>
   <si>
     <t>This doesn't round correctly, for 100.25T should read 221160lbs, needs to round to the nearest 10lbs.</t>
@@ -89,9 +113,6 @@
     <t>No data is entered if user does nor complete the screen</t>
   </si>
   <si>
-    <t>done?</t>
-  </si>
-  <si>
     <t>The back button in the explorer window should not load the page again.</t>
   </si>
   <si>
@@ -104,7 +125,10 @@
     <t>Rail car:</t>
   </si>
   <si>
-    <t>Weight on arrival should show “Weight on arrival in Tons”, “Weight at origin in Tons” Needs to allow for two decimal’s .</t>
+    <t>railcars;</t>
+  </si>
+  <si>
+    <t>Done – converted to decimal</t>
   </si>
   <si>
     <t>Errored out / not approved.</t>
@@ -141,6 +165,9 @@
   </si>
   <si>
     <t>DB</t>
+  </si>
+  <si>
+    <t>done- automatically done by Rails and sql</t>
   </si>
   <si>
     <t>UI needs to be a little more pretty.</t>
@@ -240,7 +267,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -271,6 +298,13 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -385,35 +419,35 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -440,8 +474,8 @@
   </sheetPr>
   <dimension ref="1:36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -3560,7 +3594,7 @@
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="52.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -3568,11 +3602,11 @@
         <v>5</v>
       </c>
       <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
-        <v>7</v>
+      <c r="D4" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="0"/>
       <c r="G4" s="0"/>
@@ -4596,13 +4630,13 @@
     </row>
     <row r="5" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>7</v>
@@ -5632,13 +5666,13 @@
     </row>
     <row r="6" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>7</v>
@@ -6668,17 +6702,17 @@
     </row>
     <row r="7" customFormat="false" ht="105.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7" s="0"/>
       <c r="G7" s="0"/>
@@ -7702,16 +7736,16 @@
     </row>
     <row r="8" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>25</v>
@@ -8746,7 +8780,9 @@
       <c r="C9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
@@ -11822,7 +11858,7 @@
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
         <v>29</v>
       </c>
@@ -11832,11 +11868,11 @@
       <c r="C12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>7</v>
+      <c r="D12" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
@@ -12860,19 +12896,19 @@
     </row>
     <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
@@ -13896,17 +13932,17 @@
     </row>
     <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
@@ -14930,19 +14966,19 @@
     </row>
     <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F15" s="0"/>
       <c r="G15" s="0"/>
@@ -15966,19 +16002,19 @@
     </row>
     <row r="16" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
@@ -17002,17 +17038,17 @@
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
@@ -18034,17 +18070,19 @@
       <c r="AMI17" s="0"/>
       <c r="AMJ17" s="0"/>
     </row>
-    <row r="18" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="E18" s="7"/>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
@@ -19068,17 +19106,17 @@
     </row>
     <row r="19" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F19" s="0"/>
       <c r="G19" s="0"/>
@@ -20102,13 +20140,13 @@
     </row>
     <row r="20" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>7</v>
@@ -21136,19 +21174,19 @@
     </row>
     <row r="21" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F21" s="0"/>
       <c r="G21" s="0"/>
@@ -22172,7 +22210,7 @@
     </row>
     <row r="22" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B22" s="16"/>
       <c r="C22" s="17"/>
@@ -24228,7 +24266,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -25256,17 +25294,17 @@
     </row>
     <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F25" s="0"/>
       <c r="G25" s="0"/>
@@ -26290,10 +26328,10 @@
     </row>
     <row r="26" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10" t="s">
@@ -27324,7 +27362,7 @@
     </row>
     <row r="27" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>5</v>
@@ -28354,17 +28392,17 @@
     </row>
     <row r="28" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F28" s="0"/>
       <c r="G28" s="0"/>
@@ -29388,13 +29426,13 @@
     </row>
     <row r="29" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="7"/>
@@ -30420,13 +30458,13 @@
     </row>
     <row r="30" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="7"/>
@@ -31452,7 +31490,7 @@
     </row>
     <row r="31" customFormat="false" ht="52.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>5</v>
@@ -32482,13 +32520,13 @@
     </row>
     <row r="32" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="7"/>
@@ -33514,19 +33552,19 @@
     </row>
     <row r="33" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
@@ -34550,13 +34588,13 @@
     </row>
     <row r="34" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>7</v>
@@ -34565,7 +34603,7 @@
     </row>
     <row r="35" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>5</v>
@@ -34576,13 +34614,13 @@
     </row>
     <row r="36" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
added functionality to subtract updated remaining weights based on trailer weight entered. weight on PO are now read only
</commit_message>
<xml_diff>
--- a/Requirements/m2w initial feedback.xlsx
+++ b/Requirements/m2w initial feedback.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
   <si>
     <t>Purchase Order screen:</t>
   </si>
@@ -62,7 +62,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>th</t>
     </r>
@@ -71,7 +70,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t> decimal – done</t>
     </r>
@@ -101,7 +99,7 @@
     <t>difficult</t>
   </si>
   <si>
-    <t>I'll have to check the Access DB how this is done</t>
+    <t>I'll have to check the Access DB how this is done. Completed added functionality that weight cannot be changed on updates and can only be entered, otherwise remaining weight does not match.</t>
   </si>
   <si>
     <t>Calculation is PO# Tonnage - Trailered Tons = Remaining weight</t>
@@ -110,7 +108,7 @@
     <t>Not allow for the user to click the back button, I need it to crash/not load a screen.</t>
   </si>
   <si>
-    <t>No data is entered if user does nor complete the screen</t>
+    <t>No data is entered if user does nor complete the screen.  </t>
   </si>
   <si>
     <t>The back button in the explorer window should not load the page again.</t>
@@ -122,10 +120,25 @@
     <t>check if all the fields are handled</t>
   </si>
   <si>
+    <t>make po_nbr a foreign key</t>
+  </si>
+  <si>
+    <t>speed up searches by po nbr</t>
+  </si>
+  <si>
+    <t>make remaining_weight_tons a foreign key</t>
+  </si>
+  <si>
+    <t>PO # needs to be big int</t>
+  </si>
+  <si>
+    <t>reg integer is too small</t>
+  </si>
+  <si>
     <t>Rail car:</t>
   </si>
   <si>
-    <t>railcars;</t>
+    <t>Weight on arrival should show “Weight on arrival in Tons”, “Weight at origin in Tons” Needs to allow for two decimal’s .</t>
   </si>
   <si>
     <t>Done – converted to decimal</t>
@@ -161,10 +174,13 @@
     <t>Purchase order should be a drop down from those PO's that have a remanining balance &gt; 100 lbs</t>
   </si>
   <si>
-    <t>Any remaining weight on the PO &gt;100lbs (.5T) display the PO in the drop down.'</t>
+    <t>rema</t>
   </si>
   <si>
     <t>DB</t>
+  </si>
+  <si>
+    <t>No data is entered if user does nor complete the screen</t>
   </si>
   <si>
     <t>done- automatically done by Rails and sql</t>
@@ -259,6 +275,12 @@
   <si>
     <t>Once I figure out how to do it for Rail Car, I can use the same logic</t>
   </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>display messages on screens rather than logs, like record not found</t>
+  </si>
 </sst>
 </file>
 
@@ -267,12 +289,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -294,20 +315,23 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val=""/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -315,7 +339,6 @@
       <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -323,7 +346,6 @@
       <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -374,7 +396,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -420,39 +442,47 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -472,10 +502,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:36"/>
+  <dimension ref="1:42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -6700,7 +6730,7 @@
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="105.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
         <v>19</v>
       </c>
@@ -6710,7 +6740,9 @@
       <c r="C7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E7" s="7" t="s">
         <v>22</v>
       </c>
@@ -7734,7 +7766,7 @@
       <c r="AMI7" s="0"/>
       <c r="AMJ7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>23</v>
       </c>
@@ -9804,10 +9836,16 @@
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="D10" s="10"/>
       <c r="E10" s="8"/>
       <c r="F10" s="0"/>
@@ -10830,14 +10868,18 @@
       <c r="AMI10" s="0"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>28</v>
+    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
+        <v>30</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="D11" s="10"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
       <c r="H11" s="0"/>
@@ -11858,22 +11900,18 @@
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>29</v>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>10</v>
+      <c r="C12" s="10" t="s">
+        <v>32</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>31</v>
-      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
       <c r="H12" s="0"/>
@@ -12894,22 +12932,14 @@
       <c r="AMI12" s="0"/>
       <c r="AMJ12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="7" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
@@ -13930,19 +13960,21 @@
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>33</v>
+      <c r="E14" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
@@ -14964,21 +14996,21 @@
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
-    <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F15" s="0"/>
       <c r="G15" s="0"/>
@@ -16000,21 +16032,19 @@
       <c r="AMI15" s="0"/>
       <c r="AMJ15" s="0"/>
     </row>
-    <row r="16" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>33</v>
+      <c r="E16" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
@@ -17036,19 +17066,21 @@
       <c r="AMI16" s="0"/>
       <c r="AMJ16" s="0"/>
     </row>
-    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E17" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
@@ -18070,20 +18102,22 @@
       <c r="AMI17" s="0"/>
       <c r="AMJ17" s="0"/>
     </row>
-    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>24</v>
+      <c r="C18" s="10" t="s">
+        <v>44</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>43</v>
+      <c r="D18" s="10" t="s">
+        <v>7</v>
       </c>
-      <c r="E18" s="7"/>
+      <c r="E18" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
@@ -19104,19 +19138,19 @@
       <c r="AMI18" s="0"/>
       <c r="AMJ18" s="0"/>
     </row>
-    <row r="19" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="B19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="F19" s="0"/>
       <c r="G19" s="0"/>
@@ -20138,18 +20172,18 @@
       <c r="AMI19" s="0"/>
       <c r="AMJ19" s="0"/>
     </row>
-    <row r="20" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="D20" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>7</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="0"/>
@@ -21172,21 +21206,19 @@
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
     </row>
-    <row r="21" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="s">
+    <row r="21" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="13" t="s">
+      <c r="B21" s="10"/>
+      <c r="C21" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>7</v>
+      <c r="D21" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="F21" s="0"/>
       <c r="G21" s="0"/>
@@ -22209,15 +22241,19 @@
       <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="s">
-        <v>52</v>
+      <c r="A22" s="8" t="s">
+        <v>54</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18" t="s">
+      <c r="B22" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="19"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="0"/>
       <c r="G22" s="0"/>
       <c r="H22" s="0"/>
@@ -23239,11 +23275,21 @@
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="8"/>
+      <c r="A23" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="F23" s="0"/>
       <c r="G23" s="0"/>
       <c r="H23" s="0"/>
@@ -24264,14 +24310,16 @@
       <c r="AMI23" s="0"/>
       <c r="AMJ23" s="0"/>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>53</v>
+    <row r="24" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="16" t="s">
+        <v>58</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="7"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="20"/>
       <c r="F24" s="0"/>
       <c r="G24" s="0"/>
       <c r="H24" s="0"/>
@@ -25293,19 +25341,11 @@
       <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="A25" s="10"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="10"/>
-      <c r="D25" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="8"/>
       <c r="F25" s="0"/>
       <c r="G25" s="0"/>
       <c r="H25" s="0"/>
@@ -26326,20 +26366,14 @@
       <c r="AMI25" s="0"/>
       <c r="AMJ25" s="0"/>
     </row>
-    <row r="26" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
-        <v>56</v>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>59</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="B26" s="10"/>
       <c r="C26" s="10"/>
-      <c r="D26" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="0"/>
       <c r="G26" s="0"/>
       <c r="H26" s="0"/>
@@ -27360,16 +27394,20 @@
       <c r="AMI26" s="0"/>
       <c r="AMJ26" s="0"/>
     </row>
-    <row r="27" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="7"/>
+      <c r="D27" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="F27" s="0"/>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
@@ -28390,19 +28428,19 @@
       <c r="AMI27" s="0"/>
       <c r="AMJ27" s="0"/>
     </row>
-    <row r="28" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>33</v>
+      <c r="E28" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="F28" s="0"/>
       <c r="G28" s="0"/>
@@ -29424,16 +29462,14 @@
       <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
     </row>
-    <row r="29" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="7"/>
       <c r="F29" s="0"/>
@@ -30458,16 +30494,18 @@
     </row>
     <row r="30" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>62</v>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>7</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="7"/>
+      <c r="E30" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="F30" s="0"/>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
@@ -31488,16 +31526,18 @@
       <c r="AMI30" s="0"/>
       <c r="AMJ30" s="0"/>
     </row>
-    <row r="31" customFormat="false" ht="52.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="D31" s="10"/>
-      <c r="E31" s="8"/>
+      <c r="E31" s="7"/>
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
       <c r="H31" s="0"/>
@@ -32520,13 +32560,13 @@
     </row>
     <row r="32" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="7"/>
@@ -33550,22 +33590,16 @@
       <c r="AMI32" s="0"/>
       <c r="AMJ32" s="0"/>
     </row>
-    <row r="33" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="52.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>69</v>
-      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="8"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
       <c r="H33" s="0"/>
@@ -34594,27 +34628,2069 @@
         <v>5</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>7</v>
-      </c>
+      <c r="D34" s="10"/>
       <c r="E34" s="7"/>
+      <c r="F34" s="0"/>
+      <c r="G34" s="0"/>
+      <c r="H34" s="0"/>
+      <c r="I34" s="0"/>
+      <c r="J34" s="0"/>
+      <c r="K34" s="0"/>
+      <c r="L34" s="0"/>
+      <c r="M34" s="0"/>
+      <c r="N34" s="0"/>
+      <c r="O34" s="0"/>
+      <c r="P34" s="0"/>
+      <c r="Q34" s="0"/>
+      <c r="R34" s="0"/>
+      <c r="S34" s="0"/>
+      <c r="T34" s="0"/>
+      <c r="U34" s="0"/>
+      <c r="V34" s="0"/>
+      <c r="W34" s="0"/>
+      <c r="X34" s="0"/>
+      <c r="Y34" s="0"/>
+      <c r="Z34" s="0"/>
+      <c r="AA34" s="0"/>
+      <c r="AB34" s="0"/>
+      <c r="AC34" s="0"/>
+      <c r="AD34" s="0"/>
+      <c r="AE34" s="0"/>
+      <c r="AF34" s="0"/>
+      <c r="AG34" s="0"/>
+      <c r="AH34" s="0"/>
+      <c r="AI34" s="0"/>
+      <c r="AJ34" s="0"/>
+      <c r="AK34" s="0"/>
+      <c r="AL34" s="0"/>
+      <c r="AM34" s="0"/>
+      <c r="AN34" s="0"/>
+      <c r="AO34" s="0"/>
+      <c r="AP34" s="0"/>
+      <c r="AQ34" s="0"/>
+      <c r="AR34" s="0"/>
+      <c r="AS34" s="0"/>
+      <c r="AT34" s="0"/>
+      <c r="AU34" s="0"/>
+      <c r="AV34" s="0"/>
+      <c r="AW34" s="0"/>
+      <c r="AX34" s="0"/>
+      <c r="AY34" s="0"/>
+      <c r="AZ34" s="0"/>
+      <c r="BA34" s="0"/>
+      <c r="BB34" s="0"/>
+      <c r="BC34" s="0"/>
+      <c r="BD34" s="0"/>
+      <c r="BE34" s="0"/>
+      <c r="BF34" s="0"/>
+      <c r="BG34" s="0"/>
+      <c r="BH34" s="0"/>
+      <c r="BI34" s="0"/>
+      <c r="BJ34" s="0"/>
+      <c r="BK34" s="0"/>
+      <c r="BL34" s="0"/>
+      <c r="BM34" s="0"/>
+      <c r="BN34" s="0"/>
+      <c r="BO34" s="0"/>
+      <c r="BP34" s="0"/>
+      <c r="BQ34" s="0"/>
+      <c r="BR34" s="0"/>
+      <c r="BS34" s="0"/>
+      <c r="BT34" s="0"/>
+      <c r="BU34" s="0"/>
+      <c r="BV34" s="0"/>
+      <c r="BW34" s="0"/>
+      <c r="BX34" s="0"/>
+      <c r="BY34" s="0"/>
+      <c r="BZ34" s="0"/>
+      <c r="CA34" s="0"/>
+      <c r="CB34" s="0"/>
+      <c r="CC34" s="0"/>
+      <c r="CD34" s="0"/>
+      <c r="CE34" s="0"/>
+      <c r="CF34" s="0"/>
+      <c r="CG34" s="0"/>
+      <c r="CH34" s="0"/>
+      <c r="CI34" s="0"/>
+      <c r="CJ34" s="0"/>
+      <c r="CK34" s="0"/>
+      <c r="CL34" s="0"/>
+      <c r="CM34" s="0"/>
+      <c r="CN34" s="0"/>
+      <c r="CO34" s="0"/>
+      <c r="CP34" s="0"/>
+      <c r="CQ34" s="0"/>
+      <c r="CR34" s="0"/>
+      <c r="CS34" s="0"/>
+      <c r="CT34" s="0"/>
+      <c r="CU34" s="0"/>
+      <c r="CV34" s="0"/>
+      <c r="CW34" s="0"/>
+      <c r="CX34" s="0"/>
+      <c r="CY34" s="0"/>
+      <c r="CZ34" s="0"/>
+      <c r="DA34" s="0"/>
+      <c r="DB34" s="0"/>
+      <c r="DC34" s="0"/>
+      <c r="DD34" s="0"/>
+      <c r="DE34" s="0"/>
+      <c r="DF34" s="0"/>
+      <c r="DG34" s="0"/>
+      <c r="DH34" s="0"/>
+      <c r="DI34" s="0"/>
+      <c r="DJ34" s="0"/>
+      <c r="DK34" s="0"/>
+      <c r="DL34" s="0"/>
+      <c r="DM34" s="0"/>
+      <c r="DN34" s="0"/>
+      <c r="DO34" s="0"/>
+      <c r="DP34" s="0"/>
+      <c r="DQ34" s="0"/>
+      <c r="DR34" s="0"/>
+      <c r="DS34" s="0"/>
+      <c r="DT34" s="0"/>
+      <c r="DU34" s="0"/>
+      <c r="DV34" s="0"/>
+      <c r="DW34" s="0"/>
+      <c r="DX34" s="0"/>
+      <c r="DY34" s="0"/>
+      <c r="DZ34" s="0"/>
+      <c r="EA34" s="0"/>
+      <c r="EB34" s="0"/>
+      <c r="EC34" s="0"/>
+      <c r="ED34" s="0"/>
+      <c r="EE34" s="0"/>
+      <c r="EF34" s="0"/>
+      <c r="EG34" s="0"/>
+      <c r="EH34" s="0"/>
+      <c r="EI34" s="0"/>
+      <c r="EJ34" s="0"/>
+      <c r="EK34" s="0"/>
+      <c r="EL34" s="0"/>
+      <c r="EM34" s="0"/>
+      <c r="EN34" s="0"/>
+      <c r="EO34" s="0"/>
+      <c r="EP34" s="0"/>
+      <c r="EQ34" s="0"/>
+      <c r="ER34" s="0"/>
+      <c r="ES34" s="0"/>
+      <c r="ET34" s="0"/>
+      <c r="EU34" s="0"/>
+      <c r="EV34" s="0"/>
+      <c r="EW34" s="0"/>
+      <c r="EX34" s="0"/>
+      <c r="EY34" s="0"/>
+      <c r="EZ34" s="0"/>
+      <c r="FA34" s="0"/>
+      <c r="FB34" s="0"/>
+      <c r="FC34" s="0"/>
+      <c r="FD34" s="0"/>
+      <c r="FE34" s="0"/>
+      <c r="FF34" s="0"/>
+      <c r="FG34" s="0"/>
+      <c r="FH34" s="0"/>
+      <c r="FI34" s="0"/>
+      <c r="FJ34" s="0"/>
+      <c r="FK34" s="0"/>
+      <c r="FL34" s="0"/>
+      <c r="FM34" s="0"/>
+      <c r="FN34" s="0"/>
+      <c r="FO34" s="0"/>
+      <c r="FP34" s="0"/>
+      <c r="FQ34" s="0"/>
+      <c r="FR34" s="0"/>
+      <c r="FS34" s="0"/>
+      <c r="FT34" s="0"/>
+      <c r="FU34" s="0"/>
+      <c r="FV34" s="0"/>
+      <c r="FW34" s="0"/>
+      <c r="FX34" s="0"/>
+      <c r="FY34" s="0"/>
+      <c r="FZ34" s="0"/>
+      <c r="GA34" s="0"/>
+      <c r="GB34" s="0"/>
+      <c r="GC34" s="0"/>
+      <c r="GD34" s="0"/>
+      <c r="GE34" s="0"/>
+      <c r="GF34" s="0"/>
+      <c r="GG34" s="0"/>
+      <c r="GH34" s="0"/>
+      <c r="GI34" s="0"/>
+      <c r="GJ34" s="0"/>
+      <c r="GK34" s="0"/>
+      <c r="GL34" s="0"/>
+      <c r="GM34" s="0"/>
+      <c r="GN34" s="0"/>
+      <c r="GO34" s="0"/>
+      <c r="GP34" s="0"/>
+      <c r="GQ34" s="0"/>
+      <c r="GR34" s="0"/>
+      <c r="GS34" s="0"/>
+      <c r="GT34" s="0"/>
+      <c r="GU34" s="0"/>
+      <c r="GV34" s="0"/>
+      <c r="GW34" s="0"/>
+      <c r="GX34" s="0"/>
+      <c r="GY34" s="0"/>
+      <c r="GZ34" s="0"/>
+      <c r="HA34" s="0"/>
+      <c r="HB34" s="0"/>
+      <c r="HC34" s="0"/>
+      <c r="HD34" s="0"/>
+      <c r="HE34" s="0"/>
+      <c r="HF34" s="0"/>
+      <c r="HG34" s="0"/>
+      <c r="HH34" s="0"/>
+      <c r="HI34" s="0"/>
+      <c r="HJ34" s="0"/>
+      <c r="HK34" s="0"/>
+      <c r="HL34" s="0"/>
+      <c r="HM34" s="0"/>
+      <c r="HN34" s="0"/>
+      <c r="HO34" s="0"/>
+      <c r="HP34" s="0"/>
+      <c r="HQ34" s="0"/>
+      <c r="HR34" s="0"/>
+      <c r="HS34" s="0"/>
+      <c r="HT34" s="0"/>
+      <c r="HU34" s="0"/>
+      <c r="HV34" s="0"/>
+      <c r="HW34" s="0"/>
+      <c r="HX34" s="0"/>
+      <c r="HY34" s="0"/>
+      <c r="HZ34" s="0"/>
+      <c r="IA34" s="0"/>
+      <c r="IB34" s="0"/>
+      <c r="IC34" s="0"/>
+      <c r="ID34" s="0"/>
+      <c r="IE34" s="0"/>
+      <c r="IF34" s="0"/>
+      <c r="IG34" s="0"/>
+      <c r="IH34" s="0"/>
+      <c r="II34" s="0"/>
+      <c r="IJ34" s="0"/>
+      <c r="IK34" s="0"/>
+      <c r="IL34" s="0"/>
+      <c r="IM34" s="0"/>
+      <c r="IN34" s="0"/>
+      <c r="IO34" s="0"/>
+      <c r="IP34" s="0"/>
+      <c r="IQ34" s="0"/>
+      <c r="IR34" s="0"/>
+      <c r="IS34" s="0"/>
+      <c r="IT34" s="0"/>
+      <c r="IU34" s="0"/>
+      <c r="IV34" s="0"/>
+      <c r="IW34" s="0"/>
+      <c r="IX34" s="0"/>
+      <c r="IY34" s="0"/>
+      <c r="IZ34" s="0"/>
+      <c r="JA34" s="0"/>
+      <c r="JB34" s="0"/>
+      <c r="JC34" s="0"/>
+      <c r="JD34" s="0"/>
+      <c r="JE34" s="0"/>
+      <c r="JF34" s="0"/>
+      <c r="JG34" s="0"/>
+      <c r="JH34" s="0"/>
+      <c r="JI34" s="0"/>
+      <c r="JJ34" s="0"/>
+      <c r="JK34" s="0"/>
+      <c r="JL34" s="0"/>
+      <c r="JM34" s="0"/>
+      <c r="JN34" s="0"/>
+      <c r="JO34" s="0"/>
+      <c r="JP34" s="0"/>
+      <c r="JQ34" s="0"/>
+      <c r="JR34" s="0"/>
+      <c r="JS34" s="0"/>
+      <c r="JT34" s="0"/>
+      <c r="JU34" s="0"/>
+      <c r="JV34" s="0"/>
+      <c r="JW34" s="0"/>
+      <c r="JX34" s="0"/>
+      <c r="JY34" s="0"/>
+      <c r="JZ34" s="0"/>
+      <c r="KA34" s="0"/>
+      <c r="KB34" s="0"/>
+      <c r="KC34" s="0"/>
+      <c r="KD34" s="0"/>
+      <c r="KE34" s="0"/>
+      <c r="KF34" s="0"/>
+      <c r="KG34" s="0"/>
+      <c r="KH34" s="0"/>
+      <c r="KI34" s="0"/>
+      <c r="KJ34" s="0"/>
+      <c r="KK34" s="0"/>
+      <c r="KL34" s="0"/>
+      <c r="KM34" s="0"/>
+      <c r="KN34" s="0"/>
+      <c r="KO34" s="0"/>
+      <c r="KP34" s="0"/>
+      <c r="KQ34" s="0"/>
+      <c r="KR34" s="0"/>
+      <c r="KS34" s="0"/>
+      <c r="KT34" s="0"/>
+      <c r="KU34" s="0"/>
+      <c r="KV34" s="0"/>
+      <c r="KW34" s="0"/>
+      <c r="KX34" s="0"/>
+      <c r="KY34" s="0"/>
+      <c r="KZ34" s="0"/>
+      <c r="LA34" s="0"/>
+      <c r="LB34" s="0"/>
+      <c r="LC34" s="0"/>
+      <c r="LD34" s="0"/>
+      <c r="LE34" s="0"/>
+      <c r="LF34" s="0"/>
+      <c r="LG34" s="0"/>
+      <c r="LH34" s="0"/>
+      <c r="LI34" s="0"/>
+      <c r="LJ34" s="0"/>
+      <c r="LK34" s="0"/>
+      <c r="LL34" s="0"/>
+      <c r="LM34" s="0"/>
+      <c r="LN34" s="0"/>
+      <c r="LO34" s="0"/>
+      <c r="LP34" s="0"/>
+      <c r="LQ34" s="0"/>
+      <c r="LR34" s="0"/>
+      <c r="LS34" s="0"/>
+      <c r="LT34" s="0"/>
+      <c r="LU34" s="0"/>
+      <c r="LV34" s="0"/>
+      <c r="LW34" s="0"/>
+      <c r="LX34" s="0"/>
+      <c r="LY34" s="0"/>
+      <c r="LZ34" s="0"/>
+      <c r="MA34" s="0"/>
+      <c r="MB34" s="0"/>
+      <c r="MC34" s="0"/>
+      <c r="MD34" s="0"/>
+      <c r="ME34" s="0"/>
+      <c r="MF34" s="0"/>
+      <c r="MG34" s="0"/>
+      <c r="MH34" s="0"/>
+      <c r="MI34" s="0"/>
+      <c r="MJ34" s="0"/>
+      <c r="MK34" s="0"/>
+      <c r="ML34" s="0"/>
+      <c r="MM34" s="0"/>
+      <c r="MN34" s="0"/>
+      <c r="MO34" s="0"/>
+      <c r="MP34" s="0"/>
+      <c r="MQ34" s="0"/>
+      <c r="MR34" s="0"/>
+      <c r="MS34" s="0"/>
+      <c r="MT34" s="0"/>
+      <c r="MU34" s="0"/>
+      <c r="MV34" s="0"/>
+      <c r="MW34" s="0"/>
+      <c r="MX34" s="0"/>
+      <c r="MY34" s="0"/>
+      <c r="MZ34" s="0"/>
+      <c r="NA34" s="0"/>
+      <c r="NB34" s="0"/>
+      <c r="NC34" s="0"/>
+      <c r="ND34" s="0"/>
+      <c r="NE34" s="0"/>
+      <c r="NF34" s="0"/>
+      <c r="NG34" s="0"/>
+      <c r="NH34" s="0"/>
+      <c r="NI34" s="0"/>
+      <c r="NJ34" s="0"/>
+      <c r="NK34" s="0"/>
+      <c r="NL34" s="0"/>
+      <c r="NM34" s="0"/>
+      <c r="NN34" s="0"/>
+      <c r="NO34" s="0"/>
+      <c r="NP34" s="0"/>
+      <c r="NQ34" s="0"/>
+      <c r="NR34" s="0"/>
+      <c r="NS34" s="0"/>
+      <c r="NT34" s="0"/>
+      <c r="NU34" s="0"/>
+      <c r="NV34" s="0"/>
+      <c r="NW34" s="0"/>
+      <c r="NX34" s="0"/>
+      <c r="NY34" s="0"/>
+      <c r="NZ34" s="0"/>
+      <c r="OA34" s="0"/>
+      <c r="OB34" s="0"/>
+      <c r="OC34" s="0"/>
+      <c r="OD34" s="0"/>
+      <c r="OE34" s="0"/>
+      <c r="OF34" s="0"/>
+      <c r="OG34" s="0"/>
+      <c r="OH34" s="0"/>
+      <c r="OI34" s="0"/>
+      <c r="OJ34" s="0"/>
+      <c r="OK34" s="0"/>
+      <c r="OL34" s="0"/>
+      <c r="OM34" s="0"/>
+      <c r="ON34" s="0"/>
+      <c r="OO34" s="0"/>
+      <c r="OP34" s="0"/>
+      <c r="OQ34" s="0"/>
+      <c r="OR34" s="0"/>
+      <c r="OS34" s="0"/>
+      <c r="OT34" s="0"/>
+      <c r="OU34" s="0"/>
+      <c r="OV34" s="0"/>
+      <c r="OW34" s="0"/>
+      <c r="OX34" s="0"/>
+      <c r="OY34" s="0"/>
+      <c r="OZ34" s="0"/>
+      <c r="PA34" s="0"/>
+      <c r="PB34" s="0"/>
+      <c r="PC34" s="0"/>
+      <c r="PD34" s="0"/>
+      <c r="PE34" s="0"/>
+      <c r="PF34" s="0"/>
+      <c r="PG34" s="0"/>
+      <c r="PH34" s="0"/>
+      <c r="PI34" s="0"/>
+      <c r="PJ34" s="0"/>
+      <c r="PK34" s="0"/>
+      <c r="PL34" s="0"/>
+      <c r="PM34" s="0"/>
+      <c r="PN34" s="0"/>
+      <c r="PO34" s="0"/>
+      <c r="PP34" s="0"/>
+      <c r="PQ34" s="0"/>
+      <c r="PR34" s="0"/>
+      <c r="PS34" s="0"/>
+      <c r="PT34" s="0"/>
+      <c r="PU34" s="0"/>
+      <c r="PV34" s="0"/>
+      <c r="PW34" s="0"/>
+      <c r="PX34" s="0"/>
+      <c r="PY34" s="0"/>
+      <c r="PZ34" s="0"/>
+      <c r="QA34" s="0"/>
+      <c r="QB34" s="0"/>
+      <c r="QC34" s="0"/>
+      <c r="QD34" s="0"/>
+      <c r="QE34" s="0"/>
+      <c r="QF34" s="0"/>
+      <c r="QG34" s="0"/>
+      <c r="QH34" s="0"/>
+      <c r="QI34" s="0"/>
+      <c r="QJ34" s="0"/>
+      <c r="QK34" s="0"/>
+      <c r="QL34" s="0"/>
+      <c r="QM34" s="0"/>
+      <c r="QN34" s="0"/>
+      <c r="QO34" s="0"/>
+      <c r="QP34" s="0"/>
+      <c r="QQ34" s="0"/>
+      <c r="QR34" s="0"/>
+      <c r="QS34" s="0"/>
+      <c r="QT34" s="0"/>
+      <c r="QU34" s="0"/>
+      <c r="QV34" s="0"/>
+      <c r="QW34" s="0"/>
+      <c r="QX34" s="0"/>
+      <c r="QY34" s="0"/>
+      <c r="QZ34" s="0"/>
+      <c r="RA34" s="0"/>
+      <c r="RB34" s="0"/>
+      <c r="RC34" s="0"/>
+      <c r="RD34" s="0"/>
+      <c r="RE34" s="0"/>
+      <c r="RF34" s="0"/>
+      <c r="RG34" s="0"/>
+      <c r="RH34" s="0"/>
+      <c r="RI34" s="0"/>
+      <c r="RJ34" s="0"/>
+      <c r="RK34" s="0"/>
+      <c r="RL34" s="0"/>
+      <c r="RM34" s="0"/>
+      <c r="RN34" s="0"/>
+      <c r="RO34" s="0"/>
+      <c r="RP34" s="0"/>
+      <c r="RQ34" s="0"/>
+      <c r="RR34" s="0"/>
+      <c r="RS34" s="0"/>
+      <c r="RT34" s="0"/>
+      <c r="RU34" s="0"/>
+      <c r="RV34" s="0"/>
+      <c r="RW34" s="0"/>
+      <c r="RX34" s="0"/>
+      <c r="RY34" s="0"/>
+      <c r="RZ34" s="0"/>
+      <c r="SA34" s="0"/>
+      <c r="SB34" s="0"/>
+      <c r="SC34" s="0"/>
+      <c r="SD34" s="0"/>
+      <c r="SE34" s="0"/>
+      <c r="SF34" s="0"/>
+      <c r="SG34" s="0"/>
+      <c r="SH34" s="0"/>
+      <c r="SI34" s="0"/>
+      <c r="SJ34" s="0"/>
+      <c r="SK34" s="0"/>
+      <c r="SL34" s="0"/>
+      <c r="SM34" s="0"/>
+      <c r="SN34" s="0"/>
+      <c r="SO34" s="0"/>
+      <c r="SP34" s="0"/>
+      <c r="SQ34" s="0"/>
+      <c r="SR34" s="0"/>
+      <c r="SS34" s="0"/>
+      <c r="ST34" s="0"/>
+      <c r="SU34" s="0"/>
+      <c r="SV34" s="0"/>
+      <c r="SW34" s="0"/>
+      <c r="SX34" s="0"/>
+      <c r="SY34" s="0"/>
+      <c r="SZ34" s="0"/>
+      <c r="TA34" s="0"/>
+      <c r="TB34" s="0"/>
+      <c r="TC34" s="0"/>
+      <c r="TD34" s="0"/>
+      <c r="TE34" s="0"/>
+      <c r="TF34" s="0"/>
+      <c r="TG34" s="0"/>
+      <c r="TH34" s="0"/>
+      <c r="TI34" s="0"/>
+      <c r="TJ34" s="0"/>
+      <c r="TK34" s="0"/>
+      <c r="TL34" s="0"/>
+      <c r="TM34" s="0"/>
+      <c r="TN34" s="0"/>
+      <c r="TO34" s="0"/>
+      <c r="TP34" s="0"/>
+      <c r="TQ34" s="0"/>
+      <c r="TR34" s="0"/>
+      <c r="TS34" s="0"/>
+      <c r="TT34" s="0"/>
+      <c r="TU34" s="0"/>
+      <c r="TV34" s="0"/>
+      <c r="TW34" s="0"/>
+      <c r="TX34" s="0"/>
+      <c r="TY34" s="0"/>
+      <c r="TZ34" s="0"/>
+      <c r="UA34" s="0"/>
+      <c r="UB34" s="0"/>
+      <c r="UC34" s="0"/>
+      <c r="UD34" s="0"/>
+      <c r="UE34" s="0"/>
+      <c r="UF34" s="0"/>
+      <c r="UG34" s="0"/>
+      <c r="UH34" s="0"/>
+      <c r="UI34" s="0"/>
+      <c r="UJ34" s="0"/>
+      <c r="UK34" s="0"/>
+      <c r="UL34" s="0"/>
+      <c r="UM34" s="0"/>
+      <c r="UN34" s="0"/>
+      <c r="UO34" s="0"/>
+      <c r="UP34" s="0"/>
+      <c r="UQ34" s="0"/>
+      <c r="UR34" s="0"/>
+      <c r="US34" s="0"/>
+      <c r="UT34" s="0"/>
+      <c r="UU34" s="0"/>
+      <c r="UV34" s="0"/>
+      <c r="UW34" s="0"/>
+      <c r="UX34" s="0"/>
+      <c r="UY34" s="0"/>
+      <c r="UZ34" s="0"/>
+      <c r="VA34" s="0"/>
+      <c r="VB34" s="0"/>
+      <c r="VC34" s="0"/>
+      <c r="VD34" s="0"/>
+      <c r="VE34" s="0"/>
+      <c r="VF34" s="0"/>
+      <c r="VG34" s="0"/>
+      <c r="VH34" s="0"/>
+      <c r="VI34" s="0"/>
+      <c r="VJ34" s="0"/>
+      <c r="VK34" s="0"/>
+      <c r="VL34" s="0"/>
+      <c r="VM34" s="0"/>
+      <c r="VN34" s="0"/>
+      <c r="VO34" s="0"/>
+      <c r="VP34" s="0"/>
+      <c r="VQ34" s="0"/>
+      <c r="VR34" s="0"/>
+      <c r="VS34" s="0"/>
+      <c r="VT34" s="0"/>
+      <c r="VU34" s="0"/>
+      <c r="VV34" s="0"/>
+      <c r="VW34" s="0"/>
+      <c r="VX34" s="0"/>
+      <c r="VY34" s="0"/>
+      <c r="VZ34" s="0"/>
+      <c r="WA34" s="0"/>
+      <c r="WB34" s="0"/>
+      <c r="WC34" s="0"/>
+      <c r="WD34" s="0"/>
+      <c r="WE34" s="0"/>
+      <c r="WF34" s="0"/>
+      <c r="WG34" s="0"/>
+      <c r="WH34" s="0"/>
+      <c r="WI34" s="0"/>
+      <c r="WJ34" s="0"/>
+      <c r="WK34" s="0"/>
+      <c r="WL34" s="0"/>
+      <c r="WM34" s="0"/>
+      <c r="WN34" s="0"/>
+      <c r="WO34" s="0"/>
+      <c r="WP34" s="0"/>
+      <c r="WQ34" s="0"/>
+      <c r="WR34" s="0"/>
+      <c r="WS34" s="0"/>
+      <c r="WT34" s="0"/>
+      <c r="WU34" s="0"/>
+      <c r="WV34" s="0"/>
+      <c r="WW34" s="0"/>
+      <c r="WX34" s="0"/>
+      <c r="WY34" s="0"/>
+      <c r="WZ34" s="0"/>
+      <c r="XA34" s="0"/>
+      <c r="XB34" s="0"/>
+      <c r="XC34" s="0"/>
+      <c r="XD34" s="0"/>
+      <c r="XE34" s="0"/>
+      <c r="XF34" s="0"/>
+      <c r="XG34" s="0"/>
+      <c r="XH34" s="0"/>
+      <c r="XI34" s="0"/>
+      <c r="XJ34" s="0"/>
+      <c r="XK34" s="0"/>
+      <c r="XL34" s="0"/>
+      <c r="XM34" s="0"/>
+      <c r="XN34" s="0"/>
+      <c r="XO34" s="0"/>
+      <c r="XP34" s="0"/>
+      <c r="XQ34" s="0"/>
+      <c r="XR34" s="0"/>
+      <c r="XS34" s="0"/>
+      <c r="XT34" s="0"/>
+      <c r="XU34" s="0"/>
+      <c r="XV34" s="0"/>
+      <c r="XW34" s="0"/>
+      <c r="XX34" s="0"/>
+      <c r="XY34" s="0"/>
+      <c r="XZ34" s="0"/>
+      <c r="YA34" s="0"/>
+      <c r="YB34" s="0"/>
+      <c r="YC34" s="0"/>
+      <c r="YD34" s="0"/>
+      <c r="YE34" s="0"/>
+      <c r="YF34" s="0"/>
+      <c r="YG34" s="0"/>
+      <c r="YH34" s="0"/>
+      <c r="YI34" s="0"/>
+      <c r="YJ34" s="0"/>
+      <c r="YK34" s="0"/>
+      <c r="YL34" s="0"/>
+      <c r="YM34" s="0"/>
+      <c r="YN34" s="0"/>
+      <c r="YO34" s="0"/>
+      <c r="YP34" s="0"/>
+      <c r="YQ34" s="0"/>
+      <c r="YR34" s="0"/>
+      <c r="YS34" s="0"/>
+      <c r="YT34" s="0"/>
+      <c r="YU34" s="0"/>
+      <c r="YV34" s="0"/>
+      <c r="YW34" s="0"/>
+      <c r="YX34" s="0"/>
+      <c r="YY34" s="0"/>
+      <c r="YZ34" s="0"/>
+      <c r="ZA34" s="0"/>
+      <c r="ZB34" s="0"/>
+      <c r="ZC34" s="0"/>
+      <c r="ZD34" s="0"/>
+      <c r="ZE34" s="0"/>
+      <c r="ZF34" s="0"/>
+      <c r="ZG34" s="0"/>
+      <c r="ZH34" s="0"/>
+      <c r="ZI34" s="0"/>
+      <c r="ZJ34" s="0"/>
+      <c r="ZK34" s="0"/>
+      <c r="ZL34" s="0"/>
+      <c r="ZM34" s="0"/>
+      <c r="ZN34" s="0"/>
+      <c r="ZO34" s="0"/>
+      <c r="ZP34" s="0"/>
+      <c r="ZQ34" s="0"/>
+      <c r="ZR34" s="0"/>
+      <c r="ZS34" s="0"/>
+      <c r="ZT34" s="0"/>
+      <c r="ZU34" s="0"/>
+      <c r="ZV34" s="0"/>
+      <c r="ZW34" s="0"/>
+      <c r="ZX34" s="0"/>
+      <c r="ZY34" s="0"/>
+      <c r="ZZ34" s="0"/>
+      <c r="AAA34" s="0"/>
+      <c r="AAB34" s="0"/>
+      <c r="AAC34" s="0"/>
+      <c r="AAD34" s="0"/>
+      <c r="AAE34" s="0"/>
+      <c r="AAF34" s="0"/>
+      <c r="AAG34" s="0"/>
+      <c r="AAH34" s="0"/>
+      <c r="AAI34" s="0"/>
+      <c r="AAJ34" s="0"/>
+      <c r="AAK34" s="0"/>
+      <c r="AAL34" s="0"/>
+      <c r="AAM34" s="0"/>
+      <c r="AAN34" s="0"/>
+      <c r="AAO34" s="0"/>
+      <c r="AAP34" s="0"/>
+      <c r="AAQ34" s="0"/>
+      <c r="AAR34" s="0"/>
+      <c r="AAS34" s="0"/>
+      <c r="AAT34" s="0"/>
+      <c r="AAU34" s="0"/>
+      <c r="AAV34" s="0"/>
+      <c r="AAW34" s="0"/>
+      <c r="AAX34" s="0"/>
+      <c r="AAY34" s="0"/>
+      <c r="AAZ34" s="0"/>
+      <c r="ABA34" s="0"/>
+      <c r="ABB34" s="0"/>
+      <c r="ABC34" s="0"/>
+      <c r="ABD34" s="0"/>
+      <c r="ABE34" s="0"/>
+      <c r="ABF34" s="0"/>
+      <c r="ABG34" s="0"/>
+      <c r="ABH34" s="0"/>
+      <c r="ABI34" s="0"/>
+      <c r="ABJ34" s="0"/>
+      <c r="ABK34" s="0"/>
+      <c r="ABL34" s="0"/>
+      <c r="ABM34" s="0"/>
+      <c r="ABN34" s="0"/>
+      <c r="ABO34" s="0"/>
+      <c r="ABP34" s="0"/>
+      <c r="ABQ34" s="0"/>
+      <c r="ABR34" s="0"/>
+      <c r="ABS34" s="0"/>
+      <c r="ABT34" s="0"/>
+      <c r="ABU34" s="0"/>
+      <c r="ABV34" s="0"/>
+      <c r="ABW34" s="0"/>
+      <c r="ABX34" s="0"/>
+      <c r="ABY34" s="0"/>
+      <c r="ABZ34" s="0"/>
+      <c r="ACA34" s="0"/>
+      <c r="ACB34" s="0"/>
+      <c r="ACC34" s="0"/>
+      <c r="ACD34" s="0"/>
+      <c r="ACE34" s="0"/>
+      <c r="ACF34" s="0"/>
+      <c r="ACG34" s="0"/>
+      <c r="ACH34" s="0"/>
+      <c r="ACI34" s="0"/>
+      <c r="ACJ34" s="0"/>
+      <c r="ACK34" s="0"/>
+      <c r="ACL34" s="0"/>
+      <c r="ACM34" s="0"/>
+      <c r="ACN34" s="0"/>
+      <c r="ACO34" s="0"/>
+      <c r="ACP34" s="0"/>
+      <c r="ACQ34" s="0"/>
+      <c r="ACR34" s="0"/>
+      <c r="ACS34" s="0"/>
+      <c r="ACT34" s="0"/>
+      <c r="ACU34" s="0"/>
+      <c r="ACV34" s="0"/>
+      <c r="ACW34" s="0"/>
+      <c r="ACX34" s="0"/>
+      <c r="ACY34" s="0"/>
+      <c r="ACZ34" s="0"/>
+      <c r="ADA34" s="0"/>
+      <c r="ADB34" s="0"/>
+      <c r="ADC34" s="0"/>
+      <c r="ADD34" s="0"/>
+      <c r="ADE34" s="0"/>
+      <c r="ADF34" s="0"/>
+      <c r="ADG34" s="0"/>
+      <c r="ADH34" s="0"/>
+      <c r="ADI34" s="0"/>
+      <c r="ADJ34" s="0"/>
+      <c r="ADK34" s="0"/>
+      <c r="ADL34" s="0"/>
+      <c r="ADM34" s="0"/>
+      <c r="ADN34" s="0"/>
+      <c r="ADO34" s="0"/>
+      <c r="ADP34" s="0"/>
+      <c r="ADQ34" s="0"/>
+      <c r="ADR34" s="0"/>
+      <c r="ADS34" s="0"/>
+      <c r="ADT34" s="0"/>
+      <c r="ADU34" s="0"/>
+      <c r="ADV34" s="0"/>
+      <c r="ADW34" s="0"/>
+      <c r="ADX34" s="0"/>
+      <c r="ADY34" s="0"/>
+      <c r="ADZ34" s="0"/>
+      <c r="AEA34" s="0"/>
+      <c r="AEB34" s="0"/>
+      <c r="AEC34" s="0"/>
+      <c r="AED34" s="0"/>
+      <c r="AEE34" s="0"/>
+      <c r="AEF34" s="0"/>
+      <c r="AEG34" s="0"/>
+      <c r="AEH34" s="0"/>
+      <c r="AEI34" s="0"/>
+      <c r="AEJ34" s="0"/>
+      <c r="AEK34" s="0"/>
+      <c r="AEL34" s="0"/>
+      <c r="AEM34" s="0"/>
+      <c r="AEN34" s="0"/>
+      <c r="AEO34" s="0"/>
+      <c r="AEP34" s="0"/>
+      <c r="AEQ34" s="0"/>
+      <c r="AER34" s="0"/>
+      <c r="AES34" s="0"/>
+      <c r="AET34" s="0"/>
+      <c r="AEU34" s="0"/>
+      <c r="AEV34" s="0"/>
+      <c r="AEW34" s="0"/>
+      <c r="AEX34" s="0"/>
+      <c r="AEY34" s="0"/>
+      <c r="AEZ34" s="0"/>
+      <c r="AFA34" s="0"/>
+      <c r="AFB34" s="0"/>
+      <c r="AFC34" s="0"/>
+      <c r="AFD34" s="0"/>
+      <c r="AFE34" s="0"/>
+      <c r="AFF34" s="0"/>
+      <c r="AFG34" s="0"/>
+      <c r="AFH34" s="0"/>
+      <c r="AFI34" s="0"/>
+      <c r="AFJ34" s="0"/>
+      <c r="AFK34" s="0"/>
+      <c r="AFL34" s="0"/>
+      <c r="AFM34" s="0"/>
+      <c r="AFN34" s="0"/>
+      <c r="AFO34" s="0"/>
+      <c r="AFP34" s="0"/>
+      <c r="AFQ34" s="0"/>
+      <c r="AFR34" s="0"/>
+      <c r="AFS34" s="0"/>
+      <c r="AFT34" s="0"/>
+      <c r="AFU34" s="0"/>
+      <c r="AFV34" s="0"/>
+      <c r="AFW34" s="0"/>
+      <c r="AFX34" s="0"/>
+      <c r="AFY34" s="0"/>
+      <c r="AFZ34" s="0"/>
+      <c r="AGA34" s="0"/>
+      <c r="AGB34" s="0"/>
+      <c r="AGC34" s="0"/>
+      <c r="AGD34" s="0"/>
+      <c r="AGE34" s="0"/>
+      <c r="AGF34" s="0"/>
+      <c r="AGG34" s="0"/>
+      <c r="AGH34" s="0"/>
+      <c r="AGI34" s="0"/>
+      <c r="AGJ34" s="0"/>
+      <c r="AGK34" s="0"/>
+      <c r="AGL34" s="0"/>
+      <c r="AGM34" s="0"/>
+      <c r="AGN34" s="0"/>
+      <c r="AGO34" s="0"/>
+      <c r="AGP34" s="0"/>
+      <c r="AGQ34" s="0"/>
+      <c r="AGR34" s="0"/>
+      <c r="AGS34" s="0"/>
+      <c r="AGT34" s="0"/>
+      <c r="AGU34" s="0"/>
+      <c r="AGV34" s="0"/>
+      <c r="AGW34" s="0"/>
+      <c r="AGX34" s="0"/>
+      <c r="AGY34" s="0"/>
+      <c r="AGZ34" s="0"/>
+      <c r="AHA34" s="0"/>
+      <c r="AHB34" s="0"/>
+      <c r="AHC34" s="0"/>
+      <c r="AHD34" s="0"/>
+      <c r="AHE34" s="0"/>
+      <c r="AHF34" s="0"/>
+      <c r="AHG34" s="0"/>
+      <c r="AHH34" s="0"/>
+      <c r="AHI34" s="0"/>
+      <c r="AHJ34" s="0"/>
+      <c r="AHK34" s="0"/>
+      <c r="AHL34" s="0"/>
+      <c r="AHM34" s="0"/>
+      <c r="AHN34" s="0"/>
+      <c r="AHO34" s="0"/>
+      <c r="AHP34" s="0"/>
+      <c r="AHQ34" s="0"/>
+      <c r="AHR34" s="0"/>
+      <c r="AHS34" s="0"/>
+      <c r="AHT34" s="0"/>
+      <c r="AHU34" s="0"/>
+      <c r="AHV34" s="0"/>
+      <c r="AHW34" s="0"/>
+      <c r="AHX34" s="0"/>
+      <c r="AHY34" s="0"/>
+      <c r="AHZ34" s="0"/>
+      <c r="AIA34" s="0"/>
+      <c r="AIB34" s="0"/>
+      <c r="AIC34" s="0"/>
+      <c r="AID34" s="0"/>
+      <c r="AIE34" s="0"/>
+      <c r="AIF34" s="0"/>
+      <c r="AIG34" s="0"/>
+      <c r="AIH34" s="0"/>
+      <c r="AII34" s="0"/>
+      <c r="AIJ34" s="0"/>
+      <c r="AIK34" s="0"/>
+      <c r="AIL34" s="0"/>
+      <c r="AIM34" s="0"/>
+      <c r="AIN34" s="0"/>
+      <c r="AIO34" s="0"/>
+      <c r="AIP34" s="0"/>
+      <c r="AIQ34" s="0"/>
+      <c r="AIR34" s="0"/>
+      <c r="AIS34" s="0"/>
+      <c r="AIT34" s="0"/>
+      <c r="AIU34" s="0"/>
+      <c r="AIV34" s="0"/>
+      <c r="AIW34" s="0"/>
+      <c r="AIX34" s="0"/>
+      <c r="AIY34" s="0"/>
+      <c r="AIZ34" s="0"/>
+      <c r="AJA34" s="0"/>
+      <c r="AJB34" s="0"/>
+      <c r="AJC34" s="0"/>
+      <c r="AJD34" s="0"/>
+      <c r="AJE34" s="0"/>
+      <c r="AJF34" s="0"/>
+      <c r="AJG34" s="0"/>
+      <c r="AJH34" s="0"/>
+      <c r="AJI34" s="0"/>
+      <c r="AJJ34" s="0"/>
+      <c r="AJK34" s="0"/>
+      <c r="AJL34" s="0"/>
+      <c r="AJM34" s="0"/>
+      <c r="AJN34" s="0"/>
+      <c r="AJO34" s="0"/>
+      <c r="AJP34" s="0"/>
+      <c r="AJQ34" s="0"/>
+      <c r="AJR34" s="0"/>
+      <c r="AJS34" s="0"/>
+      <c r="AJT34" s="0"/>
+      <c r="AJU34" s="0"/>
+      <c r="AJV34" s="0"/>
+      <c r="AJW34" s="0"/>
+      <c r="AJX34" s="0"/>
+      <c r="AJY34" s="0"/>
+      <c r="AJZ34" s="0"/>
+      <c r="AKA34" s="0"/>
+      <c r="AKB34" s="0"/>
+      <c r="AKC34" s="0"/>
+      <c r="AKD34" s="0"/>
+      <c r="AKE34" s="0"/>
+      <c r="AKF34" s="0"/>
+      <c r="AKG34" s="0"/>
+      <c r="AKH34" s="0"/>
+      <c r="AKI34" s="0"/>
+      <c r="AKJ34" s="0"/>
+      <c r="AKK34" s="0"/>
+      <c r="AKL34" s="0"/>
+      <c r="AKM34" s="0"/>
+      <c r="AKN34" s="0"/>
+      <c r="AKO34" s="0"/>
+      <c r="AKP34" s="0"/>
+      <c r="AKQ34" s="0"/>
+      <c r="AKR34" s="0"/>
+      <c r="AKS34" s="0"/>
+      <c r="AKT34" s="0"/>
+      <c r="AKU34" s="0"/>
+      <c r="AKV34" s="0"/>
+      <c r="AKW34" s="0"/>
+      <c r="AKX34" s="0"/>
+      <c r="AKY34" s="0"/>
+      <c r="AKZ34" s="0"/>
+      <c r="ALA34" s="0"/>
+      <c r="ALB34" s="0"/>
+      <c r="ALC34" s="0"/>
+      <c r="ALD34" s="0"/>
+      <c r="ALE34" s="0"/>
+      <c r="ALF34" s="0"/>
+      <c r="ALG34" s="0"/>
+      <c r="ALH34" s="0"/>
+      <c r="ALI34" s="0"/>
+      <c r="ALJ34" s="0"/>
+      <c r="ALK34" s="0"/>
+      <c r="ALL34" s="0"/>
+      <c r="ALM34" s="0"/>
+      <c r="ALN34" s="0"/>
+      <c r="ALO34" s="0"/>
+      <c r="ALP34" s="0"/>
+      <c r="ALQ34" s="0"/>
+      <c r="ALR34" s="0"/>
+      <c r="ALS34" s="0"/>
+      <c r="ALT34" s="0"/>
+      <c r="ALU34" s="0"/>
+      <c r="ALV34" s="0"/>
+      <c r="ALW34" s="0"/>
+      <c r="ALX34" s="0"/>
+      <c r="ALY34" s="0"/>
+      <c r="ALZ34" s="0"/>
+      <c r="AMA34" s="0"/>
+      <c r="AMB34" s="0"/>
+      <c r="AMC34" s="0"/>
+      <c r="AMD34" s="0"/>
+      <c r="AME34" s="0"/>
+      <c r="AMF34" s="0"/>
+      <c r="AMG34" s="0"/>
+      <c r="AMH34" s="0"/>
+      <c r="AMI34" s="0"/>
+      <c r="AMJ34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="8"/>
+      <c r="C35" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="0"/>
+      <c r="G35" s="0"/>
+      <c r="H35" s="0"/>
+      <c r="I35" s="0"/>
+      <c r="J35" s="0"/>
+      <c r="K35" s="0"/>
+      <c r="L35" s="0"/>
+      <c r="M35" s="0"/>
+      <c r="N35" s="0"/>
+      <c r="O35" s="0"/>
+      <c r="P35" s="0"/>
+      <c r="Q35" s="0"/>
+      <c r="R35" s="0"/>
+      <c r="S35" s="0"/>
+      <c r="T35" s="0"/>
+      <c r="U35" s="0"/>
+      <c r="V35" s="0"/>
+      <c r="W35" s="0"/>
+      <c r="X35" s="0"/>
+      <c r="Y35" s="0"/>
+      <c r="Z35" s="0"/>
+      <c r="AA35" s="0"/>
+      <c r="AB35" s="0"/>
+      <c r="AC35" s="0"/>
+      <c r="AD35" s="0"/>
+      <c r="AE35" s="0"/>
+      <c r="AF35" s="0"/>
+      <c r="AG35" s="0"/>
+      <c r="AH35" s="0"/>
+      <c r="AI35" s="0"/>
+      <c r="AJ35" s="0"/>
+      <c r="AK35" s="0"/>
+      <c r="AL35" s="0"/>
+      <c r="AM35" s="0"/>
+      <c r="AN35" s="0"/>
+      <c r="AO35" s="0"/>
+      <c r="AP35" s="0"/>
+      <c r="AQ35" s="0"/>
+      <c r="AR35" s="0"/>
+      <c r="AS35" s="0"/>
+      <c r="AT35" s="0"/>
+      <c r="AU35" s="0"/>
+      <c r="AV35" s="0"/>
+      <c r="AW35" s="0"/>
+      <c r="AX35" s="0"/>
+      <c r="AY35" s="0"/>
+      <c r="AZ35" s="0"/>
+      <c r="BA35" s="0"/>
+      <c r="BB35" s="0"/>
+      <c r="BC35" s="0"/>
+      <c r="BD35" s="0"/>
+      <c r="BE35" s="0"/>
+      <c r="BF35" s="0"/>
+      <c r="BG35" s="0"/>
+      <c r="BH35" s="0"/>
+      <c r="BI35" s="0"/>
+      <c r="BJ35" s="0"/>
+      <c r="BK35" s="0"/>
+      <c r="BL35" s="0"/>
+      <c r="BM35" s="0"/>
+      <c r="BN35" s="0"/>
+      <c r="BO35" s="0"/>
+      <c r="BP35" s="0"/>
+      <c r="BQ35" s="0"/>
+      <c r="BR35" s="0"/>
+      <c r="BS35" s="0"/>
+      <c r="BT35" s="0"/>
+      <c r="BU35" s="0"/>
+      <c r="BV35" s="0"/>
+      <c r="BW35" s="0"/>
+      <c r="BX35" s="0"/>
+      <c r="BY35" s="0"/>
+      <c r="BZ35" s="0"/>
+      <c r="CA35" s="0"/>
+      <c r="CB35" s="0"/>
+      <c r="CC35" s="0"/>
+      <c r="CD35" s="0"/>
+      <c r="CE35" s="0"/>
+      <c r="CF35" s="0"/>
+      <c r="CG35" s="0"/>
+      <c r="CH35" s="0"/>
+      <c r="CI35" s="0"/>
+      <c r="CJ35" s="0"/>
+      <c r="CK35" s="0"/>
+      <c r="CL35" s="0"/>
+      <c r="CM35" s="0"/>
+      <c r="CN35" s="0"/>
+      <c r="CO35" s="0"/>
+      <c r="CP35" s="0"/>
+      <c r="CQ35" s="0"/>
+      <c r="CR35" s="0"/>
+      <c r="CS35" s="0"/>
+      <c r="CT35" s="0"/>
+      <c r="CU35" s="0"/>
+      <c r="CV35" s="0"/>
+      <c r="CW35" s="0"/>
+      <c r="CX35" s="0"/>
+      <c r="CY35" s="0"/>
+      <c r="CZ35" s="0"/>
+      <c r="DA35" s="0"/>
+      <c r="DB35" s="0"/>
+      <c r="DC35" s="0"/>
+      <c r="DD35" s="0"/>
+      <c r="DE35" s="0"/>
+      <c r="DF35" s="0"/>
+      <c r="DG35" s="0"/>
+      <c r="DH35" s="0"/>
+      <c r="DI35" s="0"/>
+      <c r="DJ35" s="0"/>
+      <c r="DK35" s="0"/>
+      <c r="DL35" s="0"/>
+      <c r="DM35" s="0"/>
+      <c r="DN35" s="0"/>
+      <c r="DO35" s="0"/>
+      <c r="DP35" s="0"/>
+      <c r="DQ35" s="0"/>
+      <c r="DR35" s="0"/>
+      <c r="DS35" s="0"/>
+      <c r="DT35" s="0"/>
+      <c r="DU35" s="0"/>
+      <c r="DV35" s="0"/>
+      <c r="DW35" s="0"/>
+      <c r="DX35" s="0"/>
+      <c r="DY35" s="0"/>
+      <c r="DZ35" s="0"/>
+      <c r="EA35" s="0"/>
+      <c r="EB35" s="0"/>
+      <c r="EC35" s="0"/>
+      <c r="ED35" s="0"/>
+      <c r="EE35" s="0"/>
+      <c r="EF35" s="0"/>
+      <c r="EG35" s="0"/>
+      <c r="EH35" s="0"/>
+      <c r="EI35" s="0"/>
+      <c r="EJ35" s="0"/>
+      <c r="EK35" s="0"/>
+      <c r="EL35" s="0"/>
+      <c r="EM35" s="0"/>
+      <c r="EN35" s="0"/>
+      <c r="EO35" s="0"/>
+      <c r="EP35" s="0"/>
+      <c r="EQ35" s="0"/>
+      <c r="ER35" s="0"/>
+      <c r="ES35" s="0"/>
+      <c r="ET35" s="0"/>
+      <c r="EU35" s="0"/>
+      <c r="EV35" s="0"/>
+      <c r="EW35" s="0"/>
+      <c r="EX35" s="0"/>
+      <c r="EY35" s="0"/>
+      <c r="EZ35" s="0"/>
+      <c r="FA35" s="0"/>
+      <c r="FB35" s="0"/>
+      <c r="FC35" s="0"/>
+      <c r="FD35" s="0"/>
+      <c r="FE35" s="0"/>
+      <c r="FF35" s="0"/>
+      <c r="FG35" s="0"/>
+      <c r="FH35" s="0"/>
+      <c r="FI35" s="0"/>
+      <c r="FJ35" s="0"/>
+      <c r="FK35" s="0"/>
+      <c r="FL35" s="0"/>
+      <c r="FM35" s="0"/>
+      <c r="FN35" s="0"/>
+      <c r="FO35" s="0"/>
+      <c r="FP35" s="0"/>
+      <c r="FQ35" s="0"/>
+      <c r="FR35" s="0"/>
+      <c r="FS35" s="0"/>
+      <c r="FT35" s="0"/>
+      <c r="FU35" s="0"/>
+      <c r="FV35" s="0"/>
+      <c r="FW35" s="0"/>
+      <c r="FX35" s="0"/>
+      <c r="FY35" s="0"/>
+      <c r="FZ35" s="0"/>
+      <c r="GA35" s="0"/>
+      <c r="GB35" s="0"/>
+      <c r="GC35" s="0"/>
+      <c r="GD35" s="0"/>
+      <c r="GE35" s="0"/>
+      <c r="GF35" s="0"/>
+      <c r="GG35" s="0"/>
+      <c r="GH35" s="0"/>
+      <c r="GI35" s="0"/>
+      <c r="GJ35" s="0"/>
+      <c r="GK35" s="0"/>
+      <c r="GL35" s="0"/>
+      <c r="GM35" s="0"/>
+      <c r="GN35" s="0"/>
+      <c r="GO35" s="0"/>
+      <c r="GP35" s="0"/>
+      <c r="GQ35" s="0"/>
+      <c r="GR35" s="0"/>
+      <c r="GS35" s="0"/>
+      <c r="GT35" s="0"/>
+      <c r="GU35" s="0"/>
+      <c r="GV35" s="0"/>
+      <c r="GW35" s="0"/>
+      <c r="GX35" s="0"/>
+      <c r="GY35" s="0"/>
+      <c r="GZ35" s="0"/>
+      <c r="HA35" s="0"/>
+      <c r="HB35" s="0"/>
+      <c r="HC35" s="0"/>
+      <c r="HD35" s="0"/>
+      <c r="HE35" s="0"/>
+      <c r="HF35" s="0"/>
+      <c r="HG35" s="0"/>
+      <c r="HH35" s="0"/>
+      <c r="HI35" s="0"/>
+      <c r="HJ35" s="0"/>
+      <c r="HK35" s="0"/>
+      <c r="HL35" s="0"/>
+      <c r="HM35" s="0"/>
+      <c r="HN35" s="0"/>
+      <c r="HO35" s="0"/>
+      <c r="HP35" s="0"/>
+      <c r="HQ35" s="0"/>
+      <c r="HR35" s="0"/>
+      <c r="HS35" s="0"/>
+      <c r="HT35" s="0"/>
+      <c r="HU35" s="0"/>
+      <c r="HV35" s="0"/>
+      <c r="HW35" s="0"/>
+      <c r="HX35" s="0"/>
+      <c r="HY35" s="0"/>
+      <c r="HZ35" s="0"/>
+      <c r="IA35" s="0"/>
+      <c r="IB35" s="0"/>
+      <c r="IC35" s="0"/>
+      <c r="ID35" s="0"/>
+      <c r="IE35" s="0"/>
+      <c r="IF35" s="0"/>
+      <c r="IG35" s="0"/>
+      <c r="IH35" s="0"/>
+      <c r="II35" s="0"/>
+      <c r="IJ35" s="0"/>
+      <c r="IK35" s="0"/>
+      <c r="IL35" s="0"/>
+      <c r="IM35" s="0"/>
+      <c r="IN35" s="0"/>
+      <c r="IO35" s="0"/>
+      <c r="IP35" s="0"/>
+      <c r="IQ35" s="0"/>
+      <c r="IR35" s="0"/>
+      <c r="IS35" s="0"/>
+      <c r="IT35" s="0"/>
+      <c r="IU35" s="0"/>
+      <c r="IV35" s="0"/>
+      <c r="IW35" s="0"/>
+      <c r="IX35" s="0"/>
+      <c r="IY35" s="0"/>
+      <c r="IZ35" s="0"/>
+      <c r="JA35" s="0"/>
+      <c r="JB35" s="0"/>
+      <c r="JC35" s="0"/>
+      <c r="JD35" s="0"/>
+      <c r="JE35" s="0"/>
+      <c r="JF35" s="0"/>
+      <c r="JG35" s="0"/>
+      <c r="JH35" s="0"/>
+      <c r="JI35" s="0"/>
+      <c r="JJ35" s="0"/>
+      <c r="JK35" s="0"/>
+      <c r="JL35" s="0"/>
+      <c r="JM35" s="0"/>
+      <c r="JN35" s="0"/>
+      <c r="JO35" s="0"/>
+      <c r="JP35" s="0"/>
+      <c r="JQ35" s="0"/>
+      <c r="JR35" s="0"/>
+      <c r="JS35" s="0"/>
+      <c r="JT35" s="0"/>
+      <c r="JU35" s="0"/>
+      <c r="JV35" s="0"/>
+      <c r="JW35" s="0"/>
+      <c r="JX35" s="0"/>
+      <c r="JY35" s="0"/>
+      <c r="JZ35" s="0"/>
+      <c r="KA35" s="0"/>
+      <c r="KB35" s="0"/>
+      <c r="KC35" s="0"/>
+      <c r="KD35" s="0"/>
+      <c r="KE35" s="0"/>
+      <c r="KF35" s="0"/>
+      <c r="KG35" s="0"/>
+      <c r="KH35" s="0"/>
+      <c r="KI35" s="0"/>
+      <c r="KJ35" s="0"/>
+      <c r="KK35" s="0"/>
+      <c r="KL35" s="0"/>
+      <c r="KM35" s="0"/>
+      <c r="KN35" s="0"/>
+      <c r="KO35" s="0"/>
+      <c r="KP35" s="0"/>
+      <c r="KQ35" s="0"/>
+      <c r="KR35" s="0"/>
+      <c r="KS35" s="0"/>
+      <c r="KT35" s="0"/>
+      <c r="KU35" s="0"/>
+      <c r="KV35" s="0"/>
+      <c r="KW35" s="0"/>
+      <c r="KX35" s="0"/>
+      <c r="KY35" s="0"/>
+      <c r="KZ35" s="0"/>
+      <c r="LA35" s="0"/>
+      <c r="LB35" s="0"/>
+      <c r="LC35" s="0"/>
+      <c r="LD35" s="0"/>
+      <c r="LE35" s="0"/>
+      <c r="LF35" s="0"/>
+      <c r="LG35" s="0"/>
+      <c r="LH35" s="0"/>
+      <c r="LI35" s="0"/>
+      <c r="LJ35" s="0"/>
+      <c r="LK35" s="0"/>
+      <c r="LL35" s="0"/>
+      <c r="LM35" s="0"/>
+      <c r="LN35" s="0"/>
+      <c r="LO35" s="0"/>
+      <c r="LP35" s="0"/>
+      <c r="LQ35" s="0"/>
+      <c r="LR35" s="0"/>
+      <c r="LS35" s="0"/>
+      <c r="LT35" s="0"/>
+      <c r="LU35" s="0"/>
+      <c r="LV35" s="0"/>
+      <c r="LW35" s="0"/>
+      <c r="LX35" s="0"/>
+      <c r="LY35" s="0"/>
+      <c r="LZ35" s="0"/>
+      <c r="MA35" s="0"/>
+      <c r="MB35" s="0"/>
+      <c r="MC35" s="0"/>
+      <c r="MD35" s="0"/>
+      <c r="ME35" s="0"/>
+      <c r="MF35" s="0"/>
+      <c r="MG35" s="0"/>
+      <c r="MH35" s="0"/>
+      <c r="MI35" s="0"/>
+      <c r="MJ35" s="0"/>
+      <c r="MK35" s="0"/>
+      <c r="ML35" s="0"/>
+      <c r="MM35" s="0"/>
+      <c r="MN35" s="0"/>
+      <c r="MO35" s="0"/>
+      <c r="MP35" s="0"/>
+      <c r="MQ35" s="0"/>
+      <c r="MR35" s="0"/>
+      <c r="MS35" s="0"/>
+      <c r="MT35" s="0"/>
+      <c r="MU35" s="0"/>
+      <c r="MV35" s="0"/>
+      <c r="MW35" s="0"/>
+      <c r="MX35" s="0"/>
+      <c r="MY35" s="0"/>
+      <c r="MZ35" s="0"/>
+      <c r="NA35" s="0"/>
+      <c r="NB35" s="0"/>
+      <c r="NC35" s="0"/>
+      <c r="ND35" s="0"/>
+      <c r="NE35" s="0"/>
+      <c r="NF35" s="0"/>
+      <c r="NG35" s="0"/>
+      <c r="NH35" s="0"/>
+      <c r="NI35" s="0"/>
+      <c r="NJ35" s="0"/>
+      <c r="NK35" s="0"/>
+      <c r="NL35" s="0"/>
+      <c r="NM35" s="0"/>
+      <c r="NN35" s="0"/>
+      <c r="NO35" s="0"/>
+      <c r="NP35" s="0"/>
+      <c r="NQ35" s="0"/>
+      <c r="NR35" s="0"/>
+      <c r="NS35" s="0"/>
+      <c r="NT35" s="0"/>
+      <c r="NU35" s="0"/>
+      <c r="NV35" s="0"/>
+      <c r="NW35" s="0"/>
+      <c r="NX35" s="0"/>
+      <c r="NY35" s="0"/>
+      <c r="NZ35" s="0"/>
+      <c r="OA35" s="0"/>
+      <c r="OB35" s="0"/>
+      <c r="OC35" s="0"/>
+      <c r="OD35" s="0"/>
+      <c r="OE35" s="0"/>
+      <c r="OF35" s="0"/>
+      <c r="OG35" s="0"/>
+      <c r="OH35" s="0"/>
+      <c r="OI35" s="0"/>
+      <c r="OJ35" s="0"/>
+      <c r="OK35" s="0"/>
+      <c r="OL35" s="0"/>
+      <c r="OM35" s="0"/>
+      <c r="ON35" s="0"/>
+      <c r="OO35" s="0"/>
+      <c r="OP35" s="0"/>
+      <c r="OQ35" s="0"/>
+      <c r="OR35" s="0"/>
+      <c r="OS35" s="0"/>
+      <c r="OT35" s="0"/>
+      <c r="OU35" s="0"/>
+      <c r="OV35" s="0"/>
+      <c r="OW35" s="0"/>
+      <c r="OX35" s="0"/>
+      <c r="OY35" s="0"/>
+      <c r="OZ35" s="0"/>
+      <c r="PA35" s="0"/>
+      <c r="PB35" s="0"/>
+      <c r="PC35" s="0"/>
+      <c r="PD35" s="0"/>
+      <c r="PE35" s="0"/>
+      <c r="PF35" s="0"/>
+      <c r="PG35" s="0"/>
+      <c r="PH35" s="0"/>
+      <c r="PI35" s="0"/>
+      <c r="PJ35" s="0"/>
+      <c r="PK35" s="0"/>
+      <c r="PL35" s="0"/>
+      <c r="PM35" s="0"/>
+      <c r="PN35" s="0"/>
+      <c r="PO35" s="0"/>
+      <c r="PP35" s="0"/>
+      <c r="PQ35" s="0"/>
+      <c r="PR35" s="0"/>
+      <c r="PS35" s="0"/>
+      <c r="PT35" s="0"/>
+      <c r="PU35" s="0"/>
+      <c r="PV35" s="0"/>
+      <c r="PW35" s="0"/>
+      <c r="PX35" s="0"/>
+      <c r="PY35" s="0"/>
+      <c r="PZ35" s="0"/>
+      <c r="QA35" s="0"/>
+      <c r="QB35" s="0"/>
+      <c r="QC35" s="0"/>
+      <c r="QD35" s="0"/>
+      <c r="QE35" s="0"/>
+      <c r="QF35" s="0"/>
+      <c r="QG35" s="0"/>
+      <c r="QH35" s="0"/>
+      <c r="QI35" s="0"/>
+      <c r="QJ35" s="0"/>
+      <c r="QK35" s="0"/>
+      <c r="QL35" s="0"/>
+      <c r="QM35" s="0"/>
+      <c r="QN35" s="0"/>
+      <c r="QO35" s="0"/>
+      <c r="QP35" s="0"/>
+      <c r="QQ35" s="0"/>
+      <c r="QR35" s="0"/>
+      <c r="QS35" s="0"/>
+      <c r="QT35" s="0"/>
+      <c r="QU35" s="0"/>
+      <c r="QV35" s="0"/>
+      <c r="QW35" s="0"/>
+      <c r="QX35" s="0"/>
+      <c r="QY35" s="0"/>
+      <c r="QZ35" s="0"/>
+      <c r="RA35" s="0"/>
+      <c r="RB35" s="0"/>
+      <c r="RC35" s="0"/>
+      <c r="RD35" s="0"/>
+      <c r="RE35" s="0"/>
+      <c r="RF35" s="0"/>
+      <c r="RG35" s="0"/>
+      <c r="RH35" s="0"/>
+      <c r="RI35" s="0"/>
+      <c r="RJ35" s="0"/>
+      <c r="RK35" s="0"/>
+      <c r="RL35" s="0"/>
+      <c r="RM35" s="0"/>
+      <c r="RN35" s="0"/>
+      <c r="RO35" s="0"/>
+      <c r="RP35" s="0"/>
+      <c r="RQ35" s="0"/>
+      <c r="RR35" s="0"/>
+      <c r="RS35" s="0"/>
+      <c r="RT35" s="0"/>
+      <c r="RU35" s="0"/>
+      <c r="RV35" s="0"/>
+      <c r="RW35" s="0"/>
+      <c r="RX35" s="0"/>
+      <c r="RY35" s="0"/>
+      <c r="RZ35" s="0"/>
+      <c r="SA35" s="0"/>
+      <c r="SB35" s="0"/>
+      <c r="SC35" s="0"/>
+      <c r="SD35" s="0"/>
+      <c r="SE35" s="0"/>
+      <c r="SF35" s="0"/>
+      <c r="SG35" s="0"/>
+      <c r="SH35" s="0"/>
+      <c r="SI35" s="0"/>
+      <c r="SJ35" s="0"/>
+      <c r="SK35" s="0"/>
+      <c r="SL35" s="0"/>
+      <c r="SM35" s="0"/>
+      <c r="SN35" s="0"/>
+      <c r="SO35" s="0"/>
+      <c r="SP35" s="0"/>
+      <c r="SQ35" s="0"/>
+      <c r="SR35" s="0"/>
+      <c r="SS35" s="0"/>
+      <c r="ST35" s="0"/>
+      <c r="SU35" s="0"/>
+      <c r="SV35" s="0"/>
+      <c r="SW35" s="0"/>
+      <c r="SX35" s="0"/>
+      <c r="SY35" s="0"/>
+      <c r="SZ35" s="0"/>
+      <c r="TA35" s="0"/>
+      <c r="TB35" s="0"/>
+      <c r="TC35" s="0"/>
+      <c r="TD35" s="0"/>
+      <c r="TE35" s="0"/>
+      <c r="TF35" s="0"/>
+      <c r="TG35" s="0"/>
+      <c r="TH35" s="0"/>
+      <c r="TI35" s="0"/>
+      <c r="TJ35" s="0"/>
+      <c r="TK35" s="0"/>
+      <c r="TL35" s="0"/>
+      <c r="TM35" s="0"/>
+      <c r="TN35" s="0"/>
+      <c r="TO35" s="0"/>
+      <c r="TP35" s="0"/>
+      <c r="TQ35" s="0"/>
+      <c r="TR35" s="0"/>
+      <c r="TS35" s="0"/>
+      <c r="TT35" s="0"/>
+      <c r="TU35" s="0"/>
+      <c r="TV35" s="0"/>
+      <c r="TW35" s="0"/>
+      <c r="TX35" s="0"/>
+      <c r="TY35" s="0"/>
+      <c r="TZ35" s="0"/>
+      <c r="UA35" s="0"/>
+      <c r="UB35" s="0"/>
+      <c r="UC35" s="0"/>
+      <c r="UD35" s="0"/>
+      <c r="UE35" s="0"/>
+      <c r="UF35" s="0"/>
+      <c r="UG35" s="0"/>
+      <c r="UH35" s="0"/>
+      <c r="UI35" s="0"/>
+      <c r="UJ35" s="0"/>
+      <c r="UK35" s="0"/>
+      <c r="UL35" s="0"/>
+      <c r="UM35" s="0"/>
+      <c r="UN35" s="0"/>
+      <c r="UO35" s="0"/>
+      <c r="UP35" s="0"/>
+      <c r="UQ35" s="0"/>
+      <c r="UR35" s="0"/>
+      <c r="US35" s="0"/>
+      <c r="UT35" s="0"/>
+      <c r="UU35" s="0"/>
+      <c r="UV35" s="0"/>
+      <c r="UW35" s="0"/>
+      <c r="UX35" s="0"/>
+      <c r="UY35" s="0"/>
+      <c r="UZ35" s="0"/>
+      <c r="VA35" s="0"/>
+      <c r="VB35" s="0"/>
+      <c r="VC35" s="0"/>
+      <c r="VD35" s="0"/>
+      <c r="VE35" s="0"/>
+      <c r="VF35" s="0"/>
+      <c r="VG35" s="0"/>
+      <c r="VH35" s="0"/>
+      <c r="VI35" s="0"/>
+      <c r="VJ35" s="0"/>
+      <c r="VK35" s="0"/>
+      <c r="VL35" s="0"/>
+      <c r="VM35" s="0"/>
+      <c r="VN35" s="0"/>
+      <c r="VO35" s="0"/>
+      <c r="VP35" s="0"/>
+      <c r="VQ35" s="0"/>
+      <c r="VR35" s="0"/>
+      <c r="VS35" s="0"/>
+      <c r="VT35" s="0"/>
+      <c r="VU35" s="0"/>
+      <c r="VV35" s="0"/>
+      <c r="VW35" s="0"/>
+      <c r="VX35" s="0"/>
+      <c r="VY35" s="0"/>
+      <c r="VZ35" s="0"/>
+      <c r="WA35" s="0"/>
+      <c r="WB35" s="0"/>
+      <c r="WC35" s="0"/>
+      <c r="WD35" s="0"/>
+      <c r="WE35" s="0"/>
+      <c r="WF35" s="0"/>
+      <c r="WG35" s="0"/>
+      <c r="WH35" s="0"/>
+      <c r="WI35" s="0"/>
+      <c r="WJ35" s="0"/>
+      <c r="WK35" s="0"/>
+      <c r="WL35" s="0"/>
+      <c r="WM35" s="0"/>
+      <c r="WN35" s="0"/>
+      <c r="WO35" s="0"/>
+      <c r="WP35" s="0"/>
+      <c r="WQ35" s="0"/>
+      <c r="WR35" s="0"/>
+      <c r="WS35" s="0"/>
+      <c r="WT35" s="0"/>
+      <c r="WU35" s="0"/>
+      <c r="WV35" s="0"/>
+      <c r="WW35" s="0"/>
+      <c r="WX35" s="0"/>
+      <c r="WY35" s="0"/>
+      <c r="WZ35" s="0"/>
+      <c r="XA35" s="0"/>
+      <c r="XB35" s="0"/>
+      <c r="XC35" s="0"/>
+      <c r="XD35" s="0"/>
+      <c r="XE35" s="0"/>
+      <c r="XF35" s="0"/>
+      <c r="XG35" s="0"/>
+      <c r="XH35" s="0"/>
+      <c r="XI35" s="0"/>
+      <c r="XJ35" s="0"/>
+      <c r="XK35" s="0"/>
+      <c r="XL35" s="0"/>
+      <c r="XM35" s="0"/>
+      <c r="XN35" s="0"/>
+      <c r="XO35" s="0"/>
+      <c r="XP35" s="0"/>
+      <c r="XQ35" s="0"/>
+      <c r="XR35" s="0"/>
+      <c r="XS35" s="0"/>
+      <c r="XT35" s="0"/>
+      <c r="XU35" s="0"/>
+      <c r="XV35" s="0"/>
+      <c r="XW35" s="0"/>
+      <c r="XX35" s="0"/>
+      <c r="XY35" s="0"/>
+      <c r="XZ35" s="0"/>
+      <c r="YA35" s="0"/>
+      <c r="YB35" s="0"/>
+      <c r="YC35" s="0"/>
+      <c r="YD35" s="0"/>
+      <c r="YE35" s="0"/>
+      <c r="YF35" s="0"/>
+      <c r="YG35" s="0"/>
+      <c r="YH35" s="0"/>
+      <c r="YI35" s="0"/>
+      <c r="YJ35" s="0"/>
+      <c r="YK35" s="0"/>
+      <c r="YL35" s="0"/>
+      <c r="YM35" s="0"/>
+      <c r="YN35" s="0"/>
+      <c r="YO35" s="0"/>
+      <c r="YP35" s="0"/>
+      <c r="YQ35" s="0"/>
+      <c r="YR35" s="0"/>
+      <c r="YS35" s="0"/>
+      <c r="YT35" s="0"/>
+      <c r="YU35" s="0"/>
+      <c r="YV35" s="0"/>
+      <c r="YW35" s="0"/>
+      <c r="YX35" s="0"/>
+      <c r="YY35" s="0"/>
+      <c r="YZ35" s="0"/>
+      <c r="ZA35" s="0"/>
+      <c r="ZB35" s="0"/>
+      <c r="ZC35" s="0"/>
+      <c r="ZD35" s="0"/>
+      <c r="ZE35" s="0"/>
+      <c r="ZF35" s="0"/>
+      <c r="ZG35" s="0"/>
+      <c r="ZH35" s="0"/>
+      <c r="ZI35" s="0"/>
+      <c r="ZJ35" s="0"/>
+      <c r="ZK35" s="0"/>
+      <c r="ZL35" s="0"/>
+      <c r="ZM35" s="0"/>
+      <c r="ZN35" s="0"/>
+      <c r="ZO35" s="0"/>
+      <c r="ZP35" s="0"/>
+      <c r="ZQ35" s="0"/>
+      <c r="ZR35" s="0"/>
+      <c r="ZS35" s="0"/>
+      <c r="ZT35" s="0"/>
+      <c r="ZU35" s="0"/>
+      <c r="ZV35" s="0"/>
+      <c r="ZW35" s="0"/>
+      <c r="ZX35" s="0"/>
+      <c r="ZY35" s="0"/>
+      <c r="ZZ35" s="0"/>
+      <c r="AAA35" s="0"/>
+      <c r="AAB35" s="0"/>
+      <c r="AAC35" s="0"/>
+      <c r="AAD35" s="0"/>
+      <c r="AAE35" s="0"/>
+      <c r="AAF35" s="0"/>
+      <c r="AAG35" s="0"/>
+      <c r="AAH35" s="0"/>
+      <c r="AAI35" s="0"/>
+      <c r="AAJ35" s="0"/>
+      <c r="AAK35" s="0"/>
+      <c r="AAL35" s="0"/>
+      <c r="AAM35" s="0"/>
+      <c r="AAN35" s="0"/>
+      <c r="AAO35" s="0"/>
+      <c r="AAP35" s="0"/>
+      <c r="AAQ35" s="0"/>
+      <c r="AAR35" s="0"/>
+      <c r="AAS35" s="0"/>
+      <c r="AAT35" s="0"/>
+      <c r="AAU35" s="0"/>
+      <c r="AAV35" s="0"/>
+      <c r="AAW35" s="0"/>
+      <c r="AAX35" s="0"/>
+      <c r="AAY35" s="0"/>
+      <c r="AAZ35" s="0"/>
+      <c r="ABA35" s="0"/>
+      <c r="ABB35" s="0"/>
+      <c r="ABC35" s="0"/>
+      <c r="ABD35" s="0"/>
+      <c r="ABE35" s="0"/>
+      <c r="ABF35" s="0"/>
+      <c r="ABG35" s="0"/>
+      <c r="ABH35" s="0"/>
+      <c r="ABI35" s="0"/>
+      <c r="ABJ35" s="0"/>
+      <c r="ABK35" s="0"/>
+      <c r="ABL35" s="0"/>
+      <c r="ABM35" s="0"/>
+      <c r="ABN35" s="0"/>
+      <c r="ABO35" s="0"/>
+      <c r="ABP35" s="0"/>
+      <c r="ABQ35" s="0"/>
+      <c r="ABR35" s="0"/>
+      <c r="ABS35" s="0"/>
+      <c r="ABT35" s="0"/>
+      <c r="ABU35" s="0"/>
+      <c r="ABV35" s="0"/>
+      <c r="ABW35" s="0"/>
+      <c r="ABX35" s="0"/>
+      <c r="ABY35" s="0"/>
+      <c r="ABZ35" s="0"/>
+      <c r="ACA35" s="0"/>
+      <c r="ACB35" s="0"/>
+      <c r="ACC35" s="0"/>
+      <c r="ACD35" s="0"/>
+      <c r="ACE35" s="0"/>
+      <c r="ACF35" s="0"/>
+      <c r="ACG35" s="0"/>
+      <c r="ACH35" s="0"/>
+      <c r="ACI35" s="0"/>
+      <c r="ACJ35" s="0"/>
+      <c r="ACK35" s="0"/>
+      <c r="ACL35" s="0"/>
+      <c r="ACM35" s="0"/>
+      <c r="ACN35" s="0"/>
+      <c r="ACO35" s="0"/>
+      <c r="ACP35" s="0"/>
+      <c r="ACQ35" s="0"/>
+      <c r="ACR35" s="0"/>
+      <c r="ACS35" s="0"/>
+      <c r="ACT35" s="0"/>
+      <c r="ACU35" s="0"/>
+      <c r="ACV35" s="0"/>
+      <c r="ACW35" s="0"/>
+      <c r="ACX35" s="0"/>
+      <c r="ACY35" s="0"/>
+      <c r="ACZ35" s="0"/>
+      <c r="ADA35" s="0"/>
+      <c r="ADB35" s="0"/>
+      <c r="ADC35" s="0"/>
+      <c r="ADD35" s="0"/>
+      <c r="ADE35" s="0"/>
+      <c r="ADF35" s="0"/>
+      <c r="ADG35" s="0"/>
+      <c r="ADH35" s="0"/>
+      <c r="ADI35" s="0"/>
+      <c r="ADJ35" s="0"/>
+      <c r="ADK35" s="0"/>
+      <c r="ADL35" s="0"/>
+      <c r="ADM35" s="0"/>
+      <c r="ADN35" s="0"/>
+      <c r="ADO35" s="0"/>
+      <c r="ADP35" s="0"/>
+      <c r="ADQ35" s="0"/>
+      <c r="ADR35" s="0"/>
+      <c r="ADS35" s="0"/>
+      <c r="ADT35" s="0"/>
+      <c r="ADU35" s="0"/>
+      <c r="ADV35" s="0"/>
+      <c r="ADW35" s="0"/>
+      <c r="ADX35" s="0"/>
+      <c r="ADY35" s="0"/>
+      <c r="ADZ35" s="0"/>
+      <c r="AEA35" s="0"/>
+      <c r="AEB35" s="0"/>
+      <c r="AEC35" s="0"/>
+      <c r="AED35" s="0"/>
+      <c r="AEE35" s="0"/>
+      <c r="AEF35" s="0"/>
+      <c r="AEG35" s="0"/>
+      <c r="AEH35" s="0"/>
+      <c r="AEI35" s="0"/>
+      <c r="AEJ35" s="0"/>
+      <c r="AEK35" s="0"/>
+      <c r="AEL35" s="0"/>
+      <c r="AEM35" s="0"/>
+      <c r="AEN35" s="0"/>
+      <c r="AEO35" s="0"/>
+      <c r="AEP35" s="0"/>
+      <c r="AEQ35" s="0"/>
+      <c r="AER35" s="0"/>
+      <c r="AES35" s="0"/>
+      <c r="AET35" s="0"/>
+      <c r="AEU35" s="0"/>
+      <c r="AEV35" s="0"/>
+      <c r="AEW35" s="0"/>
+      <c r="AEX35" s="0"/>
+      <c r="AEY35" s="0"/>
+      <c r="AEZ35" s="0"/>
+      <c r="AFA35" s="0"/>
+      <c r="AFB35" s="0"/>
+      <c r="AFC35" s="0"/>
+      <c r="AFD35" s="0"/>
+      <c r="AFE35" s="0"/>
+      <c r="AFF35" s="0"/>
+      <c r="AFG35" s="0"/>
+      <c r="AFH35" s="0"/>
+      <c r="AFI35" s="0"/>
+      <c r="AFJ35" s="0"/>
+      <c r="AFK35" s="0"/>
+      <c r="AFL35" s="0"/>
+      <c r="AFM35" s="0"/>
+      <c r="AFN35" s="0"/>
+      <c r="AFO35" s="0"/>
+      <c r="AFP35" s="0"/>
+      <c r="AFQ35" s="0"/>
+      <c r="AFR35" s="0"/>
+      <c r="AFS35" s="0"/>
+      <c r="AFT35" s="0"/>
+      <c r="AFU35" s="0"/>
+      <c r="AFV35" s="0"/>
+      <c r="AFW35" s="0"/>
+      <c r="AFX35" s="0"/>
+      <c r="AFY35" s="0"/>
+      <c r="AFZ35" s="0"/>
+      <c r="AGA35" s="0"/>
+      <c r="AGB35" s="0"/>
+      <c r="AGC35" s="0"/>
+      <c r="AGD35" s="0"/>
+      <c r="AGE35" s="0"/>
+      <c r="AGF35" s="0"/>
+      <c r="AGG35" s="0"/>
+      <c r="AGH35" s="0"/>
+      <c r="AGI35" s="0"/>
+      <c r="AGJ35" s="0"/>
+      <c r="AGK35" s="0"/>
+      <c r="AGL35" s="0"/>
+      <c r="AGM35" s="0"/>
+      <c r="AGN35" s="0"/>
+      <c r="AGO35" s="0"/>
+      <c r="AGP35" s="0"/>
+      <c r="AGQ35" s="0"/>
+      <c r="AGR35" s="0"/>
+      <c r="AGS35" s="0"/>
+      <c r="AGT35" s="0"/>
+      <c r="AGU35" s="0"/>
+      <c r="AGV35" s="0"/>
+      <c r="AGW35" s="0"/>
+      <c r="AGX35" s="0"/>
+      <c r="AGY35" s="0"/>
+      <c r="AGZ35" s="0"/>
+      <c r="AHA35" s="0"/>
+      <c r="AHB35" s="0"/>
+      <c r="AHC35" s="0"/>
+      <c r="AHD35" s="0"/>
+      <c r="AHE35" s="0"/>
+      <c r="AHF35" s="0"/>
+      <c r="AHG35" s="0"/>
+      <c r="AHH35" s="0"/>
+      <c r="AHI35" s="0"/>
+      <c r="AHJ35" s="0"/>
+      <c r="AHK35" s="0"/>
+      <c r="AHL35" s="0"/>
+      <c r="AHM35" s="0"/>
+      <c r="AHN35" s="0"/>
+      <c r="AHO35" s="0"/>
+      <c r="AHP35" s="0"/>
+      <c r="AHQ35" s="0"/>
+      <c r="AHR35" s="0"/>
+      <c r="AHS35" s="0"/>
+      <c r="AHT35" s="0"/>
+      <c r="AHU35" s="0"/>
+      <c r="AHV35" s="0"/>
+      <c r="AHW35" s="0"/>
+      <c r="AHX35" s="0"/>
+      <c r="AHY35" s="0"/>
+      <c r="AHZ35" s="0"/>
+      <c r="AIA35" s="0"/>
+      <c r="AIB35" s="0"/>
+      <c r="AIC35" s="0"/>
+      <c r="AID35" s="0"/>
+      <c r="AIE35" s="0"/>
+      <c r="AIF35" s="0"/>
+      <c r="AIG35" s="0"/>
+      <c r="AIH35" s="0"/>
+      <c r="AII35" s="0"/>
+      <c r="AIJ35" s="0"/>
+      <c r="AIK35" s="0"/>
+      <c r="AIL35" s="0"/>
+      <c r="AIM35" s="0"/>
+      <c r="AIN35" s="0"/>
+      <c r="AIO35" s="0"/>
+      <c r="AIP35" s="0"/>
+      <c r="AIQ35" s="0"/>
+      <c r="AIR35" s="0"/>
+      <c r="AIS35" s="0"/>
+      <c r="AIT35" s="0"/>
+      <c r="AIU35" s="0"/>
+      <c r="AIV35" s="0"/>
+      <c r="AIW35" s="0"/>
+      <c r="AIX35" s="0"/>
+      <c r="AIY35" s="0"/>
+      <c r="AIZ35" s="0"/>
+      <c r="AJA35" s="0"/>
+      <c r="AJB35" s="0"/>
+      <c r="AJC35" s="0"/>
+      <c r="AJD35" s="0"/>
+      <c r="AJE35" s="0"/>
+      <c r="AJF35" s="0"/>
+      <c r="AJG35" s="0"/>
+      <c r="AJH35" s="0"/>
+      <c r="AJI35" s="0"/>
+      <c r="AJJ35" s="0"/>
+      <c r="AJK35" s="0"/>
+      <c r="AJL35" s="0"/>
+      <c r="AJM35" s="0"/>
+      <c r="AJN35" s="0"/>
+      <c r="AJO35" s="0"/>
+      <c r="AJP35" s="0"/>
+      <c r="AJQ35" s="0"/>
+      <c r="AJR35" s="0"/>
+      <c r="AJS35" s="0"/>
+      <c r="AJT35" s="0"/>
+      <c r="AJU35" s="0"/>
+      <c r="AJV35" s="0"/>
+      <c r="AJW35" s="0"/>
+      <c r="AJX35" s="0"/>
+      <c r="AJY35" s="0"/>
+      <c r="AJZ35" s="0"/>
+      <c r="AKA35" s="0"/>
+      <c r="AKB35" s="0"/>
+      <c r="AKC35" s="0"/>
+      <c r="AKD35" s="0"/>
+      <c r="AKE35" s="0"/>
+      <c r="AKF35" s="0"/>
+      <c r="AKG35" s="0"/>
+      <c r="AKH35" s="0"/>
+      <c r="AKI35" s="0"/>
+      <c r="AKJ35" s="0"/>
+      <c r="AKK35" s="0"/>
+      <c r="AKL35" s="0"/>
+      <c r="AKM35" s="0"/>
+      <c r="AKN35" s="0"/>
+      <c r="AKO35" s="0"/>
+      <c r="AKP35" s="0"/>
+      <c r="AKQ35" s="0"/>
+      <c r="AKR35" s="0"/>
+      <c r="AKS35" s="0"/>
+      <c r="AKT35" s="0"/>
+      <c r="AKU35" s="0"/>
+      <c r="AKV35" s="0"/>
+      <c r="AKW35" s="0"/>
+      <c r="AKX35" s="0"/>
+      <c r="AKY35" s="0"/>
+      <c r="AKZ35" s="0"/>
+      <c r="ALA35" s="0"/>
+      <c r="ALB35" s="0"/>
+      <c r="ALC35" s="0"/>
+      <c r="ALD35" s="0"/>
+      <c r="ALE35" s="0"/>
+      <c r="ALF35" s="0"/>
+      <c r="ALG35" s="0"/>
+      <c r="ALH35" s="0"/>
+      <c r="ALI35" s="0"/>
+      <c r="ALJ35" s="0"/>
+      <c r="ALK35" s="0"/>
+      <c r="ALL35" s="0"/>
+      <c r="ALM35" s="0"/>
+      <c r="ALN35" s="0"/>
+      <c r="ALO35" s="0"/>
+      <c r="ALP35" s="0"/>
+      <c r="ALQ35" s="0"/>
+      <c r="ALR35" s="0"/>
+      <c r="ALS35" s="0"/>
+      <c r="ALT35" s="0"/>
+      <c r="ALU35" s="0"/>
+      <c r="ALV35" s="0"/>
+      <c r="ALW35" s="0"/>
+      <c r="ALX35" s="0"/>
+      <c r="ALY35" s="0"/>
+      <c r="ALZ35" s="0"/>
+      <c r="AMA35" s="0"/>
+      <c r="AMB35" s="0"/>
+      <c r="AMC35" s="0"/>
+      <c r="AMD35" s="0"/>
+      <c r="AME35" s="0"/>
+      <c r="AMF35" s="0"/>
+      <c r="AMG35" s="0"/>
+      <c r="AMH35" s="0"/>
+      <c r="AMI35" s="0"/>
+      <c r="AMJ35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>5</v>
@@ -34625,7 +36701,43 @@
       <c r="D36" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E36" s="8"/>
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="8"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
modified database fields and fixed trailer-PO calculations
</commit_message>
<xml_diff>
--- a/Requirements/m2w initial feedback.xlsx
+++ b/Requirements/m2w initial feedback.xlsx
@@ -9,13 +9,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="83">
   <si>
     <t>Purchase Order screen:</t>
   </si>
@@ -176,7 +177,7 @@
     <t>Purchase order should be a drop down from those PO's that have a remanining balance &gt; 100 lbs</t>
   </si>
   <si>
-    <t>rema</t>
+    <t>Use same logic as in Trailers</t>
   </si>
   <si>
     <t>DB</t>
@@ -260,9 +261,6 @@
     <t>need to implement the same way as purchase orders with vendors</t>
   </si>
   <si>
-    <t>made weight_lbs mandatory</t>
-  </si>
-  <si>
     <t>Weight in tons should be calculated based on User entry, like with the PO Screen.</t>
   </si>
   <si>
@@ -282,6 +280,12 @@
   </si>
   <si>
     <t>display messages on screens rather than logs, like record not found</t>
+  </si>
+  <si>
+    <t>If error is encountered during create PO, cannot enter the weight</t>
+  </si>
+  <si>
+    <t>fixed logic</t>
   </si>
 </sst>
 </file>
@@ -510,10 +514,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:42"/>
+  <dimension ref="1:43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -9854,7 +9858,9 @@
       <c r="C10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
@@ -10886,7 +10892,9 @@
       <c r="C11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
@@ -11918,7 +11926,9 @@
       <c r="C12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
@@ -19154,12 +19164,10 @@
         <v>20</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D19" s="10"/>
-      <c r="E19" s="7" t="s">
-        <v>46</v>
-      </c>
+      <c r="E19" s="7"/>
       <c r="F19" s="0"/>
       <c r="G19" s="0"/>
       <c r="H19" s="0"/>
@@ -35671,10 +35679,10 @@
         <v>73</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F35" s="0"/>
       <c r="G35" s="0"/>
@@ -36696,9 +36704,9 @@
       <c r="AMI35" s="0"/>
       <c r="AMJ35" s="0"/>
     </row>
-    <row r="36" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>5</v>
@@ -36713,24 +36721,26 @@
     </row>
     <row r="37" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
+      <c r="D37" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>7</v>
@@ -36745,12 +36755,23 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
         <v>81</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -36762,4 +36783,37 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <f aca="false">LEN(1000000000)</f>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
rail cars now can be assigned to POs with weight > 100
</commit_message>
<xml_diff>
--- a/Requirements/m2w initial feedback.xlsx
+++ b/Requirements/m2w initial feedback.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="86">
   <si>
     <t>Purchase Order screen:</t>
   </si>
@@ -287,6 +287,22 @@
   <si>
     <t>fixed logic</t>
   </si>
+  <si>
+    <t>Herroku - Include 'rails_12factor' gem to enable all platform features</t>
+  </si>
+  <si>
+    <t>Herroku – You have not declared a Ruby version in your Gemfile.
+remote:        To set your Ruby version add this line to your Gemfile:
+remote:        ruby '2.0.0'
+remote:        # See https://devcenter.heroku.com/articles/ruby-versions for more information.
+</t>
+  </si>
+  <si>
+    <t>Herroku -  ###### WARNING:
+remote:        No Procfile detected, using the default web server (webrick)
+remote:        https://devcenter.heroku.com/articles/ruby-default-web-server
+</t>
+  </si>
 </sst>
 </file>
 
@@ -514,10 +530,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:43"/>
+  <dimension ref="1:46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -19166,7 +19182,9 @@
       <c r="C19" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E19" s="7"/>
       <c r="F19" s="0"/>
       <c r="G19" s="0"/>
@@ -36749,19 +36767,27 @@
     </row>
     <row r="39" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="21" t="s">
         <v>79</v>
       </c>
+      <c r="C41" s="0"/>
+      <c r="D41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
@@ -36772,6 +36798,21 @@
       </c>
       <c r="D43" s="3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enabled trailer in and out and time calculations
</commit_message>
<xml_diff>
--- a/Requirements/m2w initial feedback.xlsx
+++ b/Requirements/m2w initial feedback.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="87">
   <si>
     <t>Purchase Order screen:</t>
   </si>
@@ -291,6 +291,9 @@
     <t>Herroku - Include 'rails_12factor' gem to enable all platform features</t>
   </si>
   <si>
+    <t>added gem</t>
+  </si>
+  <si>
     <t>Herroku – You have not declared a Ruby version in your Gemfile.
 remote:        To set your Ruby version add this line to your Gemfile:
 remote:        ruby '2.0.0'
@@ -532,8 +535,8 @@
   </sheetPr>
   <dimension ref="1:46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -31570,7 +31573,9 @@
       <c r="C31" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="10"/>
+      <c r="D31" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E31" s="7"/>
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
@@ -36804,15 +36809,21 @@
       <c r="A44" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="C44" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed problem with po lbs missmatch with trailer weights
</commit_message>
<xml_diff>
--- a/Requirements/m2w initial feedback.xlsx
+++ b/Requirements/m2w initial feedback.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="87">
   <si>
     <t>Purchase Order screen:</t>
   </si>
@@ -535,8 +535,8 @@
   </sheetPr>
   <dimension ref="1:46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -33637,7 +33637,9 @@
         <v>5</v>
       </c>
       <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
+      <c r="D33" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E33" s="8"/>
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>

</xml_diff>

<commit_message>
added select rail by drop down and added PO drop down to be sorted by PO #
</commit_message>
<xml_diff>
--- a/Requirements/m2w initial feedback.xlsx
+++ b/Requirements/m2w initial feedback.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="87">
   <si>
     <t>Purchase Order screen:</t>
   </si>
@@ -32607,7 +32607,9 @@
       <c r="C32" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="10"/>
+      <c r="D32" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E32" s="7"/>
       <c r="F32" s="0"/>
       <c r="G32" s="0"/>

</xml_diff>

<commit_message>
added carrier on Trailer Edit as a drop down
</commit_message>
<xml_diff>
--- a/Requirements/m2w initial feedback.xlsx
+++ b/Requirements/m2w initial feedback.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="87">
   <si>
     <t>Purchase Order screen:</t>
   </si>
@@ -180,7 +180,7 @@
     <t>Use same logic as in Trailers</t>
   </si>
   <si>
-    <t>DB</t>
+    <t>Not allow for the user to click the back button, I need it not to crash/not load a screen</t>
   </si>
   <si>
     <t>No data is entered if user does nor complete the screen</t>
@@ -535,8 +535,8 @@
   </sheetPr>
   <dimension ref="1:46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -29507,7 +29507,9 @@
         <v>5</v>
       </c>
       <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="D29" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E29" s="7"/>
       <c r="F29" s="0"/>
       <c r="G29" s="0"/>

</xml_diff>

<commit_message>
added workers functionality and linked them to trailers
</commit_message>
<xml_diff>
--- a/Requirements/m2w initial feedback.xlsx
+++ b/Requirements/m2w initial feedback.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="87">
   <si>
     <t>Purchase Order screen:</t>
   </si>
@@ -535,8 +535,8 @@
   </sheetPr>
   <dimension ref="1:46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -34675,7 +34675,9 @@
       <c r="C34" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="10"/>
+      <c r="D34" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E34" s="7"/>
       <c r="F34" s="0"/>
       <c r="G34" s="0"/>

</xml_diff>

<commit_message>
added timeout feature and now at Beta 0
</commit_message>
<xml_diff>
--- a/Requirements/m2w initial feedback.xlsx
+++ b/Requirements/m2w initial feedback.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="90">
   <si>
     <t>Purchase Order screen:</t>
   </si>
@@ -306,6 +306,15 @@
 remote:        https://devcenter.heroku.com/articles/ruby-default-web-server
 </t>
   </si>
+  <si>
+    <t>make badge # field on trailer into a foreign key</t>
+  </si>
+  <si>
+    <t>add auto logout feature</t>
+  </si>
+  <si>
+    <t>5 minute timer</t>
+  </si>
 </sst>
 </file>
 
@@ -533,10 +542,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:46"/>
+  <dimension ref="1:48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -36834,6 +36843,22 @@
         <v>86</v>
       </c>
     </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>